<commit_message>
Now we sell eggs!
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OF\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OF\Documents\SimCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Production</t>
   </si>
@@ -215,6 +215,27 @@
   </si>
   <si>
     <t>Best price to get more utility daily</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sausages: </t>
+  </si>
+  <si>
+    <t>Eggs:</t>
+  </si>
+  <si>
+    <t>Best price to get the most utility</t>
+  </si>
+  <si>
+    <t>Revenue less wages per unit</t>
+  </si>
+  <si>
+    <t>unit production price</t>
+  </si>
+  <si>
+    <t>Units sold per hour</t>
   </si>
 </sst>
 </file>
@@ -340,6 +361,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -414,6 +436,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -796,6 +819,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -870,6 +894,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3160,7 +3185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -3512,7 +3537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -3934,507 +3959,863 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.78</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>14</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2">
-        <f>C2*60 +D2</f>
+      <c r="F2">
+        <f>D2*60 +E2</f>
         <v>850</v>
       </c>
-      <c r="F2">
-        <f>3600/E2</f>
+      <c r="G2">
+        <f>3600/F2</f>
         <v>4.2352941176470589</v>
       </c>
-      <c r="G2">
-        <f>F2*B2</f>
+      <c r="H2">
+        <f>G2*C2</f>
         <v>3.303529411764706</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.82</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>49</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E19" si="0">C3*60 +D3</f>
+      <c r="F3">
+        <f t="shared" ref="F3:F19" si="0">D3*60 +E3</f>
         <v>889</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F19" si="1">3600/E3</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G19" si="1">3600/F3</f>
         <v>4.0494938132733411</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G19" si="2">F3*B3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H19" si="2">G3*C3</f>
         <v>3.3205849268841394</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.2</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.86</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>33</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>933</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="1"/>
         <v>3.8585209003215435</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="2"/>
         <v>3.3183279742765275</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.3</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>980</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="1"/>
         <v>3.6734693877551021</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="2"/>
         <v>3.306122448979592</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.4</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.93</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>17</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>11</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>1031</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>3.4917555771096023</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="2"/>
         <v>3.2473326867119301</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.5</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.95</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>1086</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="1"/>
         <v>3.3149171270718232</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="2"/>
         <v>3.1491712707182318</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5.6</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.97</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>19</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>6</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>1146</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="1"/>
         <v>3.1413612565445028</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="2"/>
         <v>3.0471204188481678</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.7</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.99</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>20</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>1210</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="1"/>
         <v>2.9752066115702478</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="2"/>
         <v>2.9454545454545453</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.8</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>17</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>1277</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f t="shared" si="1"/>
         <v>2.8191072826938135</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="2"/>
         <v>2.8191072826938135</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5.9</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>22</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>29</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <f t="shared" si="0"/>
         <v>1349</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f t="shared" si="1"/>
         <v>2.6686434395848777</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="2"/>
         <v>2.6686434395848777</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>23</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>45</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>1425</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="1"/>
         <v>2.5263157894736841</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>2.5263157894736841</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6.1</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.99</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>25</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f t="shared" si="0"/>
         <v>1505</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f t="shared" si="1"/>
         <v>2.3920265780730898</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>2.3681063122923591</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6.2</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.98</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>26</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>29</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>1589</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <f t="shared" si="1"/>
         <v>2.2655758338577723</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>2.2202643171806167</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6.3</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.96</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>27</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>57</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>1677</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <f t="shared" si="1"/>
         <v>2.1466905187835419</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>2.0608228980322001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6.4</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.93</v>
-      </c>
-      <c r="C16">
-        <v>29</v>
       </c>
       <c r="D16">
         <v>29</v>
       </c>
       <c r="E16">
+        <v>29</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>1769</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>2.0350480497456189</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="2"/>
         <v>1.8925946862634258</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6.4999999999999902</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>0.9</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>31</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>5</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f t="shared" si="0"/>
         <v>1865</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f t="shared" si="1"/>
         <v>1.9302949061662198</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="2"/>
         <v>1.7372654155495979</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6.5999999999999899</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.87</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>32</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>45</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <f t="shared" si="0"/>
         <v>1965</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <f t="shared" si="1"/>
         <v>1.83206106870229</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="2"/>
         <v>1.5938931297709924</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6.6999999999999904</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.82</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>34</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>30</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f t="shared" si="0"/>
         <v>2070</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <f t="shared" si="1"/>
         <v>1.7391304347826086</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="2"/>
         <v>1.4260869565217391</v>
       </c>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23">
+        <f>0.933</f>
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.99</v>
+      </c>
+      <c r="B25">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C25">
+        <v>421.55</v>
+      </c>
+      <c r="D25">
+        <f>B25-$E$23</f>
+        <v>-0.3630000000000001</v>
+      </c>
+      <c r="E25">
+        <f>D25*C25</f>
+        <v>-153.02265000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="B26">
+        <v>0.72</v>
+      </c>
+      <c r="C26">
+        <v>480</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D42" si="3">B26-$E$23</f>
+        <v>-0.21300000000000008</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E38" si="4">D26*C26</f>
+        <v>-102.24000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.19</v>
+      </c>
+      <c r="B27">
+        <v>0.85</v>
+      </c>
+      <c r="C27">
+        <v>525</v>
+      </c>
+      <c r="D27">
+        <f>B27-$E$23</f>
+        <v>-8.3000000000000074E-2</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>-43.575000000000038</v>
+      </c>
+      <c r="J27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.29</v>
+      </c>
+      <c r="B28">
+        <v>0.96</v>
+      </c>
+      <c r="C28">
+        <v>544.63</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>2.6999999999999913E-2</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>14.705009999999952</v>
+      </c>
+      <c r="J28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1.39</v>
+      </c>
+      <c r="B29">
+        <v>1.06</v>
+      </c>
+      <c r="C29">
+        <v>530.97</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>0.127</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>67.43319000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1.49</v>
+      </c>
+      <c r="B30">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C30">
+        <v>490.46</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>0.19699999999999984</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>96.620619999999917</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1.59</v>
+      </c>
+      <c r="B31">
+        <v>1.18</v>
+      </c>
+      <c r="C31">
+        <v>433.21</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>0.24699999999999989</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>107.00286999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1.69</v>
+      </c>
+      <c r="B32">
+        <v>1.21</v>
+      </c>
+      <c r="C32">
+        <v>371.9</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>0.27699999999999991</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>103.01629999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.79</v>
+      </c>
+      <c r="B33">
+        <v>1.23</v>
+      </c>
+      <c r="C33">
+        <v>314.41000000000003</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>0.29699999999999993</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>93.379769999999979</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.89</v>
+      </c>
+      <c r="B34">
+        <v>1.22</v>
+      </c>
+      <c r="C34">
+        <v>264.12</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>0.28699999999999992</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>75.802439999999976</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1.99</v>
+      </c>
+      <c r="B35">
+        <v>1.19</v>
+      </c>
+      <c r="C35">
+        <v>222.09</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>0.2569999999999999</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>57.077129999999975</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2.09</v>
+      </c>
+      <c r="B36">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C36">
+        <v>187.6</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>0.21699999999999986</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>40.709199999999974</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2.19</v>
+      </c>
+      <c r="B37">
+        <v>1.08</v>
+      </c>
+      <c r="C37">
+        <v>159.5</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>0.14700000000000002</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="4"/>
+        <v>23.446500000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2.29</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>136.62</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>6.6999999999999948E-2</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="4"/>
+        <v>9.1535399999999925</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F19">
+  <conditionalFormatting sqref="G2:G19">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H19">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:G42">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H42">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4446,7 +4827,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="D25:D38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Just protected the spreadshit
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +786,7 @@
         <v>159.84</v>
       </c>
       <c r="G24" s="1">
-        <f>$E$2*F24</f>
+        <f t="shared" ref="G24:G30" si="0">$E$2*F24</f>
         <v>46.065888000000001</v>
       </c>
       <c r="H24">
@@ -815,11 +815,11 @@
         <v>65.12</v>
       </c>
       <c r="G25" s="1">
-        <f>$E$2*F25</f>
+        <f t="shared" si="0"/>
         <v>18.767584000000003</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H52" si="0">D25+F25+G25</f>
+        <f t="shared" ref="H25:H52" si="1">D25+F25+G25</f>
         <v>2158.8875840000001</v>
       </c>
     </row>
@@ -844,11 +844,11 @@
         <v>117.22</v>
       </c>
       <c r="G26" s="1">
-        <f>$E$2*F26</f>
+        <f t="shared" si="0"/>
         <v>33.782803999999999</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9601.0028039999997</v>
       </c>
     </row>
@@ -873,11 +873,11 @@
         <v>43.96</v>
       </c>
       <c r="G27" s="1">
-        <f>$E$2*F27</f>
+        <f t="shared" si="0"/>
         <v>12.669272000000001</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>510.62927199999996</v>
       </c>
     </row>
@@ -902,11 +902,11 @@
         <v>175.82</v>
       </c>
       <c r="G28" s="1">
-        <f>$E$2*F28</f>
+        <f t="shared" si="0"/>
         <v>50.671323999999998</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100543.08142400002</v>
       </c>
     </row>
@@ -931,11 +931,11 @@
         <v>351.65</v>
       </c>
       <c r="G29" s="1">
-        <f>$E$2*F29</f>
+        <f t="shared" si="0"/>
         <v>101.34553</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>619219.04662200005</v>
       </c>
     </row>
@@ -960,11 +960,11 @@
         <v>1758.23</v>
       </c>
       <c r="G30" s="1">
-        <f>$E$2*F30</f>
+        <f t="shared" si="0"/>
         <v>506.72188600000004</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>153448.52208400003</v>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
         <v>81.629768000000013</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4960.8697679999996</v>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
         <v>81.629768000000013</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5286.8697679999996</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
         <v>68.023846000000006</v>
       </c>
       <c r="H35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1392.053846</v>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
         <v>1632.56654</v>
       </c>
       <c r="H36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48695.225843999993</v>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
         <v>573.34796200000005</v>
       </c>
       <c r="H39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7262.7579619999997</v>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
         <v>573.34796200000005</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10332.757962</v>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
         <v>286.67254000000003</v>
       </c>
       <c r="H41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11410.37254</v>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
         <v>191.11694800000001</v>
       </c>
       <c r="H42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4629.2569480000002</v>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
         <v>28.667254</v>
       </c>
       <c r="H43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>549.63725399999998</v>
       </c>
     </row>
@@ -1314,7 +1314,7 @@
         <v>304.61299000000002</v>
       </c>
       <c r="H46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109167.40237600001</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
         <v>913.83897000000002</v>
       </c>
       <c r="H47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>776752.25767600012</v>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
         <v>3046.1327820000001</v>
       </c>
       <c r="H50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>220971.52147000004</v>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
         <v>1142.300874</v>
       </c>
       <c r="H51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75811.712138000003</v>
       </c>
     </row>
@@ -1450,11 +1450,12 @@
         <v>130.54883600000002</v>
       </c>
       <c r="H52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33505.058130000005</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="H24:H52">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
Plan to move to aerospace industry
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -9,10 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="5" r:id="rId1"/>
+    <sheet name="Jumbo jet" sheetId="8" r:id="rId1"/>
+    <sheet name="Luxury jet" sheetId="7" r:id="rId2"/>
+    <sheet name="s. Engine" sheetId="11" r:id="rId3"/>
+    <sheet name="BFRs" sheetId="9" r:id="rId4"/>
+    <sheet name="SORs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="71">
   <si>
     <t>Carbon composite</t>
   </si>
@@ -252,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +266,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,13 +324,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +791,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1">
@@ -795,7 +820,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="1">
@@ -824,10 +849,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -853,7 +878,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="1">
@@ -882,7 +907,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="1">
@@ -911,7 +936,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="1">
@@ -940,7 +965,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="1">
@@ -989,7 +1014,7 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="1">
@@ -1018,7 +1043,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="1">
@@ -1047,7 +1072,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="1">
@@ -1076,7 +1101,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="1">
@@ -1125,7 +1150,7 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="1">
@@ -1154,7 +1179,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1">
@@ -1183,7 +1208,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="1">
@@ -1212,7 +1237,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="1">
@@ -1290,7 +1315,7 @@
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="1">
@@ -1319,7 +1344,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="1">
@@ -1368,7 +1393,7 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="1">
@@ -1397,7 +1422,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="1">
@@ -1455,7 +1480,3542 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <conditionalFormatting sqref="H24:H52">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0.28820000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>306</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <f>40*B3</f>
+        <v>2640</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="F24" s="1">
+        <v>159.84</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G30" si="0">$E$2*F24</f>
+        <v>46.065888000000001</v>
+      </c>
+      <c r="H24">
+        <f>D24+F24+G24</f>
+        <v>2845.9058880000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <f>30*B3+5*B4</f>
+        <v>2075</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.01</v>
+      </c>
+      <c r="F25" s="1">
+        <v>65.12</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>18.767584000000003</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H52" si="1">D25+F25+G25</f>
+        <v>2158.8875840000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1">
+        <f>50*B4+250*B5</f>
+        <v>9450</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
+        <v>117.22</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>33.782803999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>9601.0028039999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <f>20*B8+30*B9</f>
+        <v>454</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="F27" s="1">
+        <v>43.96</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>12.669272000000001</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>510.62927199999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
+        <f>8*H24+2*H26+2*H33+4*H41+2*H35</f>
+        <v>100316.59010000002</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="F28" s="1">
+        <v>175.82</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>50.671323999999998</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>100543.08142400002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1">
+        <v>100</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1">
+        <f>40*H24+16*H26+34*H40</f>
+        <v>618766.05109199998</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="F29" s="1">
+        <v>351.65</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>101.34553</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>619219.04662200005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
+        <f>2*H34+10*H27+4*H35+6*H26+7*H40</f>
+        <v>151183.570198</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1758.23</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>506.72188600000004</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>153448.52208400003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="1">
+        <f>4*B10+2*B11</f>
+        <v>4596</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F33" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G33" s="1">
+        <f>$E$2*F33</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>4960.8697679999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1">
+        <f>4*B10+8*B12+B6</f>
+        <v>4922</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F34" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G34" s="1">
+        <f>$E$2*F34</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>5286.8697679999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1">
+        <f>3*B8+5*B13+3*B14</f>
+        <v>1088</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="F35" s="1">
+        <v>236.03</v>
+      </c>
+      <c r="G35" s="1">
+        <f>$E$2*F35</f>
+        <v>68.023846000000006</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1392.053846</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1">
+        <f>8*B10+4*H33+H41+2*H35</f>
+        <v>41397.959303999996</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="F36" s="1">
+        <v>5664.7</v>
+      </c>
+      <c r="G36" s="1">
+        <f>$E$2*F36</f>
+        <v>1632.56654</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>48695.225843999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1">
+        <f>30*B4+100*B5+50*B15</f>
+        <v>4700</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G39" s="1">
+        <f>$E$2*F39</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>7262.7579619999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1">
+        <f>20*B8+8*B10+10*B4</f>
+        <v>7770</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G40" s="1">
+        <f>$E$2*F40</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>10332.757962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="1">
+        <f>8*B10+30*B13+15*B15</f>
+        <v>10129</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="F41" s="1">
+        <v>994.7</v>
+      </c>
+      <c r="G41" s="1">
+        <f>$E$2*F41</f>
+        <v>286.67254000000003</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>11410.37254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="1">
+        <f>4*B10+5*B4</f>
+        <v>3775</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="F42" s="1">
+        <v>663.14</v>
+      </c>
+      <c r="G42" s="1">
+        <f>$E$2*F42</f>
+        <v>191.11694800000001</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>4629.2569480000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="1">
+        <f>6*B8+5*B15+5*B16</f>
+        <v>421.5</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.24</v>
+      </c>
+      <c r="F43" s="1">
+        <v>99.47</v>
+      </c>
+      <c r="G43" s="1">
+        <f>$E$2*F43</f>
+        <v>28.667254</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>549.63725399999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="1">
+        <f>H39+H28</f>
+        <v>107805.83938600002</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1056.95</v>
+      </c>
+      <c r="G46" s="1">
+        <f>$E$2*F46</f>
+        <v>304.61299000000002</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>109167.40237600001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="1">
+        <f>H29+H30</f>
+        <v>772667.56870600011</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3170.85</v>
+      </c>
+      <c r="G47" s="1">
+        <f>$E$2*F47</f>
+        <v>913.83897000000002</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>776752.25767600012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="1">
+        <f>40*H24+10*H25+2*H34+140*B6+4*H42</f>
+        <v>207355.87868800003</v>
+      </c>
+      <c r="E50" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>10569.51</v>
+      </c>
+      <c r="G50" s="1">
+        <f>$E$2*F50</f>
+        <v>3046.1327820000001</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>220971.52147000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="1">
+        <f>14*H24+2*H25+H34+2*B7+2*H42</f>
+        <v>70705.841264000002</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3963.57</v>
+      </c>
+      <c r="G51" s="1">
+        <f>$E$2*F51</f>
+        <v>1142.300874</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>75811.712138000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="1">
+        <f>8*H24+2*H25+H34+H43</f>
+        <v>32921.529294</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="F52" s="1">
+        <v>452.98</v>
+      </c>
+      <c r="G52" s="1">
+        <f>$E$2*F52</f>
+        <v>130.54883600000002</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>33505.058130000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H24:H52">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0.28820000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>306</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <f>40*B3</f>
+        <v>2640</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="F24" s="1">
+        <v>159.84</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G30" si="0">$E$2*F24</f>
+        <v>46.065888000000001</v>
+      </c>
+      <c r="H24">
+        <f>D24+F24+G24</f>
+        <v>2845.9058880000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <f>30*B3+5*B4</f>
+        <v>2075</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.01</v>
+      </c>
+      <c r="F25" s="1">
+        <v>65.12</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>18.767584000000003</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H52" si="1">D25+F25+G25</f>
+        <v>2158.8875840000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1">
+        <f>50*B4+250*B5</f>
+        <v>9450</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
+        <v>117.22</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>33.782803999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>9601.0028039999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <f>20*B8+30*B9</f>
+        <v>454</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="F27" s="1">
+        <v>43.96</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>12.669272000000001</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>510.62927199999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
+        <f>8*H24+2*H26+2*H33+4*H41+2*H35</f>
+        <v>100316.59010000002</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="F28" s="1">
+        <v>175.82</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>50.671323999999998</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>100543.08142400002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1">
+        <v>100</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1">
+        <f>40*H24+16*H26+34*H40</f>
+        <v>618766.05109199998</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="F29" s="1">
+        <v>351.65</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>101.34553</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>619219.04662200005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
+        <f>2*H34+10*H27+4*H35+6*H26+7*H40</f>
+        <v>151183.570198</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1758.23</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>506.72188600000004</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>153448.52208400003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="1">
+        <f>4*B10+2*B11</f>
+        <v>4596</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F33" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G33" s="1">
+        <f>$E$2*F33</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>4960.8697679999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1">
+        <f>4*B10+8*B12+B6</f>
+        <v>4922</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F34" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G34" s="1">
+        <f>$E$2*F34</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>5286.8697679999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1">
+        <f>3*B8+5*B13+3*B14</f>
+        <v>1088</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="F35" s="1">
+        <v>236.03</v>
+      </c>
+      <c r="G35" s="1">
+        <f>$E$2*F35</f>
+        <v>68.023846000000006</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1392.053846</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1">
+        <f>8*B10+4*H33+H41+2*H35</f>
+        <v>41397.959303999996</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="F36" s="1">
+        <v>5664.7</v>
+      </c>
+      <c r="G36" s="1">
+        <f>$E$2*F36</f>
+        <v>1632.56654</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>48695.225843999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1">
+        <f>30*B4+100*B5+50*B15</f>
+        <v>4700</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G39" s="1">
+        <f>$E$2*F39</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>7262.7579619999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1">
+        <f>20*B8+8*B10+10*B4</f>
+        <v>7770</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G40" s="1">
+        <f>$E$2*F40</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>10332.757962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="1">
+        <f>8*B10+30*B13+15*B15</f>
+        <v>10129</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="F41" s="1">
+        <v>994.7</v>
+      </c>
+      <c r="G41" s="1">
+        <f>$E$2*F41</f>
+        <v>286.67254000000003</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>11410.37254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="1">
+        <f>4*B10+5*B4</f>
+        <v>3775</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="F42" s="1">
+        <v>663.14</v>
+      </c>
+      <c r="G42" s="1">
+        <f>$E$2*F42</f>
+        <v>191.11694800000001</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>4629.2569480000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="1">
+        <f>6*B8+5*B15+5*B16</f>
+        <v>421.5</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.24</v>
+      </c>
+      <c r="F43" s="1">
+        <v>99.47</v>
+      </c>
+      <c r="G43" s="1">
+        <f>$E$2*F43</f>
+        <v>28.667254</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>549.63725399999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="1">
+        <f>H39+H28</f>
+        <v>107805.83938600002</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1056.95</v>
+      </c>
+      <c r="G46" s="1">
+        <f>$E$2*F46</f>
+        <v>304.61299000000002</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>109167.40237600001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="1">
+        <f>H29+H30</f>
+        <v>772667.56870600011</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3170.85</v>
+      </c>
+      <c r="G47" s="1">
+        <f>$E$2*F47</f>
+        <v>913.83897000000002</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>776752.25767600012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="1">
+        <f>40*H24+10*H25+2*H34+140*B6+4*H42</f>
+        <v>207355.87868800003</v>
+      </c>
+      <c r="E50" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>10569.51</v>
+      </c>
+      <c r="G50" s="1">
+        <f>$E$2*F50</f>
+        <v>3046.1327820000001</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>220971.52147000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="1">
+        <f>14*H24+2*H25+H34+2*B7+2*H42</f>
+        <v>70705.841264000002</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3963.57</v>
+      </c>
+      <c r="G51" s="1">
+        <f>$E$2*F51</f>
+        <v>1142.300874</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>75811.712138000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="1">
+        <f>8*H24+2*H25+H34+H43</f>
+        <v>32921.529294</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="F52" s="1">
+        <v>452.98</v>
+      </c>
+      <c r="G52" s="1">
+        <f>$E$2*F52</f>
+        <v>130.54883600000002</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>33505.058130000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H24:H52">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0.28820000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>306</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <f>40*B3</f>
+        <v>2640</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="F24" s="1">
+        <v>159.84</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G30" si="0">$E$2*F24</f>
+        <v>46.065888000000001</v>
+      </c>
+      <c r="H24">
+        <f>D24+F24+G24</f>
+        <v>2845.9058880000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <f>30*B3+5*B4</f>
+        <v>2075</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.01</v>
+      </c>
+      <c r="F25" s="1">
+        <v>65.12</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>18.767584000000003</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H52" si="1">D25+F25+G25</f>
+        <v>2158.8875840000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1">
+        <f>50*B4+250*B5</f>
+        <v>9450</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
+        <v>117.22</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>33.782803999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>9601.0028039999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <f>20*B8+30*B9</f>
+        <v>454</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="F27" s="1">
+        <v>43.96</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>12.669272000000001</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>510.62927199999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
+        <f>8*H24+2*H26+2*H33+4*H41+2*H35</f>
+        <v>100316.59010000002</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="F28" s="1">
+        <v>175.82</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>50.671323999999998</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>100543.08142400002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1">
+        <v>100</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1">
+        <f>40*H24+16*H26+34*H40</f>
+        <v>618766.05109199998</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="F29" s="1">
+        <v>351.65</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>101.34553</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>619219.04662200005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
+        <f>2*H34+10*H27+4*H35+6*H26+7*H40</f>
+        <v>151183.570198</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1758.23</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>506.72188600000004</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>153448.52208400003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="1">
+        <f>4*B10+2*B11</f>
+        <v>4596</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F33" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G33" s="1">
+        <f>$E$2*F33</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>4960.8697679999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1">
+        <f>4*B10+8*B12+B6</f>
+        <v>4922</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F34" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G34" s="1">
+        <f>$E$2*F34</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>5286.8697679999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1">
+        <f>3*B8+5*B13+3*B14</f>
+        <v>1088</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="F35" s="1">
+        <v>236.03</v>
+      </c>
+      <c r="G35" s="1">
+        <f>$E$2*F35</f>
+        <v>68.023846000000006</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1392.053846</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1">
+        <f>8*B10+4*H33+H41+2*H35</f>
+        <v>41397.959303999996</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="F36" s="1">
+        <v>5664.7</v>
+      </c>
+      <c r="G36" s="1">
+        <f>$E$2*F36</f>
+        <v>1632.56654</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>48695.225843999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1">
+        <f>30*B4+100*B5+50*B15</f>
+        <v>4700</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G39" s="1">
+        <f>$E$2*F39</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>7262.7579619999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1">
+        <f>20*B8+8*B10+10*B4</f>
+        <v>7770</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G40" s="1">
+        <f>$E$2*F40</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>10332.757962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="1">
+        <f>8*B10+30*B13+15*B15</f>
+        <v>10129</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="F41" s="1">
+        <v>994.7</v>
+      </c>
+      <c r="G41" s="1">
+        <f>$E$2*F41</f>
+        <v>286.67254000000003</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>11410.37254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="1">
+        <f>4*B10+5*B4</f>
+        <v>3775</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="F42" s="1">
+        <v>663.14</v>
+      </c>
+      <c r="G42" s="1">
+        <f>$E$2*F42</f>
+        <v>191.11694800000001</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>4629.2569480000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="1">
+        <f>6*B8+5*B15+5*B16</f>
+        <v>421.5</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.24</v>
+      </c>
+      <c r="F43" s="1">
+        <v>99.47</v>
+      </c>
+      <c r="G43" s="1">
+        <f>$E$2*F43</f>
+        <v>28.667254</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>549.63725399999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="1">
+        <f>H39+H28</f>
+        <v>107805.83938600002</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1056.95</v>
+      </c>
+      <c r="G46" s="1">
+        <f>$E$2*F46</f>
+        <v>304.61299000000002</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>109167.40237600001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="1">
+        <f>H29+H30</f>
+        <v>772667.56870600011</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3170.85</v>
+      </c>
+      <c r="G47" s="1">
+        <f>$E$2*F47</f>
+        <v>913.83897000000002</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>776752.25767600012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="1">
+        <f>40*H24+10*H25+2*H34+140*B6+4*H42</f>
+        <v>207355.87868800003</v>
+      </c>
+      <c r="E50" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>10569.51</v>
+      </c>
+      <c r="G50" s="1">
+        <f>$E$2*F50</f>
+        <v>3046.1327820000001</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>220971.52147000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="1">
+        <f>14*H24+2*H25+H34+2*B7+2*H42</f>
+        <v>70705.841264000002</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3963.57</v>
+      </c>
+      <c r="G51" s="1">
+        <f>$E$2*F51</f>
+        <v>1142.300874</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>75811.712138000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="1">
+        <f>8*H24+2*H25+H34+H43</f>
+        <v>32921.529294</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="F52" s="1">
+        <v>452.98</v>
+      </c>
+      <c r="G52" s="1">
+        <f>$E$2*F52</f>
+        <v>130.54883600000002</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>33505.058130000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H24:H52">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0.28820000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>306</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <f>40*B3</f>
+        <v>2640</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="F24" s="1">
+        <v>159.84</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G30" si="0">$E$2*F24</f>
+        <v>46.065888000000001</v>
+      </c>
+      <c r="H24">
+        <f>D24+F24+G24</f>
+        <v>2845.9058880000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <f>30*B3+5*B4</f>
+        <v>2075</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.01</v>
+      </c>
+      <c r="F25" s="1">
+        <v>65.12</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>18.767584000000003</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H52" si="1">D25+F25+G25</f>
+        <v>2158.8875840000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1">
+        <f>50*B4+250*B5</f>
+        <v>9450</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
+        <v>117.22</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>33.782803999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>9601.0028039999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <f>20*B8+30*B9</f>
+        <v>454</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="F27" s="1">
+        <v>43.96</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>12.669272000000001</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>510.62927199999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
+        <f>8*H24+2*H26+2*H33+4*H41+2*H35</f>
+        <v>100316.59010000002</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="F28" s="1">
+        <v>175.82</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>50.671323999999998</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>100543.08142400002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1">
+        <v>100</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1">
+        <f>40*H24+16*H26+34*H40</f>
+        <v>618766.05109199998</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="F29" s="1">
+        <v>351.65</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>101.34553</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>619219.04662200005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
+        <f>2*H34+10*H27+4*H35+6*H26+7*H40</f>
+        <v>151183.570198</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1758.23</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>506.72188600000004</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>153448.52208400003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="1">
+        <f>4*B10+2*B11</f>
+        <v>4596</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F33" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G33" s="1">
+        <f>$E$2*F33</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>4960.8697679999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1">
+        <f>4*B10+8*B12+B6</f>
+        <v>4922</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="F34" s="1">
+        <v>283.24</v>
+      </c>
+      <c r="G34" s="1">
+        <f>$E$2*F34</f>
+        <v>81.629768000000013</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>5286.8697679999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1">
+        <f>3*B8+5*B13+3*B14</f>
+        <v>1088</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="F35" s="1">
+        <v>236.03</v>
+      </c>
+      <c r="G35" s="1">
+        <f>$E$2*F35</f>
+        <v>68.023846000000006</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1392.053846</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1">
+        <f>8*B10+4*H33+H41+2*H35</f>
+        <v>41397.959303999996</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="F36" s="1">
+        <v>5664.7</v>
+      </c>
+      <c r="G36" s="1">
+        <f>$E$2*F36</f>
+        <v>1632.56654</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>48695.225843999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1">
+        <f>30*B4+100*B5+50*B15</f>
+        <v>4700</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G39" s="1">
+        <f>$E$2*F39</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>7262.7579619999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1">
+        <f>20*B8+8*B10+10*B4</f>
+        <v>7770</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1989.41</v>
+      </c>
+      <c r="G40" s="1">
+        <f>$E$2*F40</f>
+        <v>573.34796200000005</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>10332.757962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="1">
+        <f>8*B10+30*B13+15*B15</f>
+        <v>10129</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="F41" s="1">
+        <v>994.7</v>
+      </c>
+      <c r="G41" s="1">
+        <f>$E$2*F41</f>
+        <v>286.67254000000003</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>11410.37254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="1">
+        <f>4*B10+5*B4</f>
+        <v>3775</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="F42" s="1">
+        <v>663.14</v>
+      </c>
+      <c r="G42" s="1">
+        <f>$E$2*F42</f>
+        <v>191.11694800000001</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>4629.2569480000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="1">
+        <f>6*B8+5*B15+5*B16</f>
+        <v>421.5</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.24</v>
+      </c>
+      <c r="F43" s="1">
+        <v>99.47</v>
+      </c>
+      <c r="G43" s="1">
+        <f>$E$2*F43</f>
+        <v>28.667254</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>549.63725399999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="1">
+        <f>H39+H28</f>
+        <v>107805.83938600002</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1056.95</v>
+      </c>
+      <c r="G46" s="1">
+        <f>$E$2*F46</f>
+        <v>304.61299000000002</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>109167.40237600001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="1">
+        <f>H29+H30</f>
+        <v>772667.56870600011</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3170.85</v>
+      </c>
+      <c r="G47" s="1">
+        <f>$E$2*F47</f>
+        <v>913.83897000000002</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>776752.25767600012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="1">
+        <f>40*H24+10*H25+2*H34+140*B6+4*H42</f>
+        <v>207355.87868800003</v>
+      </c>
+      <c r="E50" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>10569.51</v>
+      </c>
+      <c r="G50" s="1">
+        <f>$E$2*F50</f>
+        <v>3046.1327820000001</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>220971.52147000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="1">
+        <f>14*H24+2*H25+H34+2*B7+2*H42</f>
+        <v>70705.841264000002</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3963.57</v>
+      </c>
+      <c r="G51" s="1">
+        <f>$E$2*F51</f>
+        <v>1142.300874</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>75811.712138000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="1">
+        <f>8*H24+2*H25+H34+H43</f>
+        <v>32921.529294</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="F52" s="1">
+        <v>452.98</v>
+      </c>
+      <c r="G52" s="1">
+        <f>$E$2*F52</f>
+        <v>130.54883600000002</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>33505.058130000005</v>
+      </c>
+    </row>
+  </sheetData>
   <conditionalFormatting sqref="H24:H52">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
VIF renting or not?
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All of them" sheetId="12" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="s. Engine" sheetId="11" r:id="rId4"/>
     <sheet name="BFRs" sheetId="9" r:id="rId5"/>
     <sheet name="SORs" sheetId="5" r:id="rId6"/>
-    <sheet name="Production Plans 1st stage" sheetId="13" r:id="rId7"/>
+    <sheet name="Rocket production" sheetId="13" r:id="rId7"/>
+    <sheet name="Production Plans second stage" sheetId="15" r:id="rId8"/>
+    <sheet name="Production Plans final stage" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="131">
   <si>
     <t>Carbon composite</t>
   </si>
@@ -332,9 +334,6 @@
     <t>NEEDS PER BFR</t>
   </si>
   <si>
-    <t>REQUIRED CASH PER BFR</t>
-  </si>
-  <si>
     <t>REQUIRED HOURS</t>
   </si>
   <si>
@@ -348,13 +347,91 @@
   </si>
   <si>
     <t>Given any slots, there's a building required level to produce the specified amount of BFR's every hour</t>
+  </si>
+  <si>
+    <t>REQUIRED CASH PER ROCKET</t>
+  </si>
+  <si>
+    <t>Level required to produce the specified amount in 1 hour with the defined amount of buildings</t>
+  </si>
+  <si>
+    <t>selling price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hourly profit </t>
+  </si>
+  <si>
+    <t>daily profit</t>
+  </si>
+  <si>
+    <t>TOTAL BUILDING LVL</t>
+  </si>
+  <si>
+    <t>selling BFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selling ASR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount per launch </t>
+  </si>
+  <si>
+    <t>probability of failure</t>
+  </si>
+  <si>
+    <t>Expected selling price</t>
+  </si>
+  <si>
+    <t>Expected hourly profit</t>
+  </si>
+  <si>
+    <t>Expected daily profit</t>
+  </si>
+  <si>
+    <t>LAUNCHPAD</t>
+  </si>
+  <si>
+    <t>1 BFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Launchpad level: </t>
+  </si>
+  <si>
+    <t>BFR with VIF rent</t>
+  </si>
+  <si>
+    <t>For the first stage we only pretend to sell BFRs</t>
+  </si>
+  <si>
+    <t>For the second stage we pretend to build a high q launchpad and sell ASR</t>
+  </si>
+  <si>
+    <t>REQUIRED CASH PER HOUR</t>
+  </si>
+  <si>
+    <t>REQUIRED CASH PER DAY</t>
+  </si>
+  <si>
+    <t>PRODUCED UNITS PER HOUR</t>
+  </si>
+  <si>
+    <t>Assuming we will prefer to launch our BFRs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assuming we can produce our own high quality BFRs. </t>
+  </si>
+  <si>
+    <t>UNITS PER HOUR PER LEVEL</t>
+  </si>
+  <si>
+    <t>daily units</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +465,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -580,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,6 +705,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5546,10 +5633,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5560,8 +5647,10 @@
     <col min="4" max="4" width="75.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5579,7 +5668,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -5588,7 +5677,7 @@
         <v>99</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="13" t="s">
@@ -5603,19 +5692,19 @@
         <v>58</v>
       </c>
       <c r="B3" s="4">
-        <f>IF(B18&gt;0,B18-1,0)</f>
+        <f>IF(B13&gt;0,B13-1,0)</f>
         <v>2</v>
       </c>
       <c r="C3" s="12">
         <v>10.5</v>
       </c>
       <c r="D3" s="4">
-        <f>20*C18</f>
-        <v>34.166666666666657</v>
+        <f>20*C13</f>
+        <v>160</v>
       </c>
       <c r="E3" s="11">
         <f>D3*C3</f>
-        <v>358.74999999999989</v>
+        <v>1680</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -5624,19 +5713,19 @@
         <v>60</v>
       </c>
       <c r="B4" s="4">
-        <f>IF(B18&gt;0,B18-1,0)</f>
+        <f>IF(B13&gt;0,B13-1,0)</f>
         <v>2</v>
       </c>
       <c r="C4" s="12">
-        <v>890</v>
+        <v>900</v>
       </c>
       <c r="D4" s="4">
-        <f>8*C18</f>
-        <v>13.666666666666664</v>
+        <f>8*C13</f>
+        <v>64</v>
       </c>
       <c r="E4" s="11">
-        <f t="shared" ref="E4:E10" si="0">D4*C4</f>
-        <v>12163.333333333332</v>
+        <f t="shared" ref="E4:E5" si="0">D4*C4</f>
+        <v>57600</v>
       </c>
       <c r="G4" s="4"/>
       <c r="K4" t="s">
@@ -5648,19 +5737,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="4">
-        <f>IF(B18&gt;0,B18-1,0)</f>
+        <f>IF(B13&gt;0,B13-1,0)</f>
         <v>2</v>
       </c>
       <c r="C5" s="12">
         <v>18.5</v>
       </c>
       <c r="D5" s="4">
-        <f>10*C18</f>
-        <v>17.083333333333329</v>
+        <f>10*C13</f>
+        <v>80</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>316.04166666666657</v>
+        <v>1480</v>
       </c>
       <c r="G5" s="4"/>
       <c r="K5" t="s">
@@ -5668,565 +5757,237 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="24">
-        <f>IF(B21&gt;0,B21-1,0)</f>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="27">
+        <f>SUM(E3:E5)</f>
+        <v>60760</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="24"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="12">
         <v>3</v>
       </c>
-      <c r="C6" s="12">
-        <v>3180</v>
-      </c>
-      <c r="D6" s="4">
-        <f>40*C21</f>
-        <v>1.6666666666666665</v>
-      </c>
-      <c r="E6" s="11">
-        <f t="shared" si="0"/>
-        <v>5299.9999999999991</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="24">
-        <f>IF(B22&gt;0,B22-1,0)</f>
-        <v>3</v>
-      </c>
-      <c r="C7" s="12">
-        <v>10300</v>
-      </c>
-      <c r="D7" s="4">
-        <f>16*C21+C22*6</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E7" s="11">
-        <f t="shared" si="0"/>
-        <v>9441.6666666666661</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="24">
-        <f>IF(B22&gt;0,B22-1,0)</f>
-        <v>3</v>
-      </c>
-      <c r="C8" s="12">
-        <v>5570</v>
-      </c>
-      <c r="D8" s="4">
-        <f>2*C22</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E8" s="11">
-        <f t="shared" si="0"/>
-        <v>464.16666666666663</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="K8" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="L8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="24">
-        <f>IF(B22&gt;0,B22-1,0)</f>
-        <v>3</v>
-      </c>
-      <c r="C9" s="12">
-        <v>545</v>
-      </c>
-      <c r="D9" s="4">
-        <f>10*C22</f>
-        <v>0.41666666666666663</v>
-      </c>
-      <c r="E9" s="11">
-        <f t="shared" si="0"/>
-        <v>227.08333333333331</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="24">
-        <f>IF(B22&gt;0,B22-1,0)</f>
-        <v>3</v>
-      </c>
-      <c r="C10" s="12">
-        <v>1730</v>
-      </c>
-      <c r="D10" s="4">
-        <f>4*C22</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="E10" s="11">
-        <f t="shared" si="0"/>
-        <v>288.33333333333331</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="27">
-        <f>SUM(E3:E10)</f>
-        <v>28559.374999999996</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="12">
+        <v>8</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="24">
+        <f>20*C3+8*C4+10*C5</f>
+        <v>7595</v>
+      </c>
+      <c r="F13" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G13" s="24">
+        <v>1989.41</v>
+      </c>
+      <c r="H13" s="24">
+        <f>$I$2*G13</f>
+        <v>278.51740000000007</v>
+      </c>
+      <c r="I13">
+        <f>C13/F13</f>
+        <v>27.586206896551726</v>
+      </c>
+      <c r="J13" s="27">
+        <f>E13+G13+H13</f>
+        <v>9862.9274000000005</v>
+      </c>
+      <c r="K13" s="24"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="40">
+        <v>9</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="39">
+        <f>I13/G14</f>
+        <v>3.0651340996168583</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="H15" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="39">
+        <f>I14*G14</f>
+        <v>27.586206896551726</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
-      <c r="B16" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" s="24"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="12">
+        <v>11700</v>
+      </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="24">
-        <f>IF(B21&gt;0,B21-1,0)</f>
-        <v>3</v>
-      </c>
-      <c r="C18" s="24">
-        <f>34*C21+7*C22</f>
-        <v>1.708333333333333</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="24">
-        <f>20*C3+8*C4+10*C5</f>
-        <v>7515</v>
-      </c>
-      <c r="F18" s="24">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G18" s="24">
-        <v>1989.41</v>
-      </c>
-      <c r="H18" s="24">
-        <f>$I$2*G18</f>
-        <v>278.51740000000007</v>
-      </c>
-      <c r="I18">
-        <f>C18/F18</f>
-        <v>5.8908045977011492</v>
-      </c>
-      <c r="J18" s="4">
-        <f>E18+G18+H18</f>
-        <v>9782.9274000000005</v>
-      </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="27">
+        <f>(C17-J13)*C13</f>
+        <v>14696.580799999996</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="28"/>
+      <c r="B19" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="27">
+        <f>C18*24</f>
+        <v>352717.93919999991</v>
+      </c>
+      <c r="D19" s="24"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="38">
-        <v>8</v>
-      </c>
-      <c r="H19" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="39">
-        <f>I18/G19</f>
-        <v>0.73635057471264365</v>
-      </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="29"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="24">
-        <f>IF(B25&gt;0,B25-1,0)</f>
-        <v>4</v>
-      </c>
-      <c r="C21" s="4">
-        <f>C25</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="4">
-        <f>40*C6+16*C7+34*J18</f>
-        <v>624619.53159999999</v>
-      </c>
-      <c r="F21" s="4">
-        <v>1.67</v>
-      </c>
-      <c r="G21" s="4">
-        <v>351.65</v>
-      </c>
-      <c r="H21" s="4">
-        <f>$I$2*G21</f>
-        <v>49.231000000000002</v>
-      </c>
-      <c r="I21">
-        <f>C21/F21</f>
-        <v>2.4950099800399202E-2</v>
-      </c>
-      <c r="J21" s="4">
-        <f>E21+G21+H21</f>
-        <v>625020.41260000004</v>
-      </c>
-      <c r="K21" s="24"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="24">
-        <f>IF(B25&gt;0,B25-1,0)</f>
-        <v>4</v>
-      </c>
-      <c r="C22" s="4">
-        <f>C25</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="4">
-        <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
-        <v>153790.49180000002</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1758.23</v>
-      </c>
-      <c r="H22" s="4">
-        <f>$I$2*G22</f>
-        <v>246.15220000000002</v>
-      </c>
-      <c r="I22">
-        <f>C22/F22</f>
-        <v>0.12626262626262624</v>
-      </c>
-      <c r="J22" s="4">
-        <f>E22+G22+H22</f>
-        <v>155794.87400000004</v>
-      </c>
-      <c r="K22" s="24"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="38">
-        <v>1</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="I23" s="39">
-        <f>(I21+I22)/G23</f>
-        <v>0.15121272606302544</v>
-      </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="12">
-        <v>5</v>
-      </c>
-      <c r="C25" s="12">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="24">
-        <f>J21+J22</f>
-        <v>780815.28660000011</v>
-      </c>
-      <c r="F25" s="24">
-        <v>0.24</v>
-      </c>
-      <c r="G25" s="24">
-        <v>3170.85</v>
-      </c>
-      <c r="H25" s="24">
-        <f>$I$2*G25</f>
-        <v>443.91900000000004</v>
-      </c>
-      <c r="I25">
-        <f>C25/F25</f>
-        <v>0.1736111111111111</v>
-      </c>
-      <c r="J25" s="24">
-        <f>E25+G25+H25</f>
-        <v>784430.05560000008</v>
-      </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="38">
-        <v>1</v>
-      </c>
-      <c r="H26" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="I26" s="39">
-        <f>I25/G26</f>
-        <v>0.1736111111111111</v>
-      </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="24"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="24"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M16:M17">
+  <conditionalFormatting sqref="M11:M12">
     <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="min"/>
@@ -6238,42 +5999,6 @@
           <x14:id>{3165805C-5004-49C5-854A-5F4767D7AE87}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:J22">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J25">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6290,6 +6015,1874 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
+          <xm:sqref>M11:M12</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="D3" s="4">
+        <f>20*C18</f>
+        <v>162.39999999999978</v>
+      </c>
+      <c r="E3" s="11">
+        <f>D3*C3</f>
+        <v>1705.1999999999978</v>
+      </c>
+      <c r="F3" s="11">
+        <f>E3*24</f>
+        <v>40924.799999999945</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>900</v>
+      </c>
+      <c r="D4" s="4">
+        <f>8*C18</f>
+        <v>64.959999999999908</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:E10" si="0">D4*C4</f>
+        <v>58463.99999999992</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" ref="F4:F10" si="1">E4*24</f>
+        <v>1403135.9999999981</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="K4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>18.5</v>
+      </c>
+      <c r="D5" s="4">
+        <f>10*C18</f>
+        <v>81.199999999999889</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>1502.199999999998</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="1"/>
+        <v>36052.799999999952</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24">
+        <f>IF(B22&gt;0,B22-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <f>3180*0.98</f>
+        <v>3116.4</v>
+      </c>
+      <c r="D6" s="4">
+        <f>40*C22</f>
+        <v>7.9219512195121844</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="0"/>
+        <v>24687.968780487772</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="1"/>
+        <v>592511.2507317065</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="12">
+        <f>9900*0.98</f>
+        <v>9702</v>
+      </c>
+      <c r="D7" s="4">
+        <f>16*C22+C23*6</f>
+        <v>4.3570731707317014</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="0"/>
+        <v>42272.32390243897</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="1"/>
+        <v>1014535.7736585352</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5570</v>
+      </c>
+      <c r="D8" s="4">
+        <f>2*C23</f>
+        <v>0.39609756097560922</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="0"/>
+        <v>2206.2634146341434</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="1"/>
+        <v>52950.321951219441</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="K8" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="12">
+        <v>545</v>
+      </c>
+      <c r="D9" s="4">
+        <f>10*C23</f>
+        <v>1.9804878048780461</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>1079.3658536585351</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>25904.780487804841</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1730</v>
+      </c>
+      <c r="D10" s="4">
+        <f>4*C23</f>
+        <v>0.79219512195121844</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="0"/>
+        <v>1370.4975609756079</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>32891.941463414594</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="27">
+        <f>SUM(E3:E10)</f>
+        <v>133287.81951219495</v>
+      </c>
+      <c r="F11" s="27">
+        <f>E11*24</f>
+        <v>3198907.6682926789</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="24"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="24">
+        <f>IF(B22&gt;0,B22-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C18" s="24">
+        <f>34*C22+7*C23</f>
+        <v>8.1199999999999886</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="24">
+        <f>20*C3+8*C4+10*C5</f>
+        <v>7595</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G18" s="24">
+        <v>1989.41</v>
+      </c>
+      <c r="H18" s="24">
+        <f>$I$2*G18</f>
+        <v>397.88200000000006</v>
+      </c>
+      <c r="I18">
+        <f>C18/F18</f>
+        <v>27.999999999999961</v>
+      </c>
+      <c r="J18" s="27">
+        <f>E18+G18+H18</f>
+        <v>9982.2919999999995</v>
+      </c>
+      <c r="K18" s="24"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="40">
+        <v>9</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="39">
+        <f>I18/G19</f>
+        <v>3.1111111111111067</v>
+      </c>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" s="39">
+        <f>I19*G19</f>
+        <v>27.999999999999961</v>
+      </c>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="24">
+        <f>IF(B27&gt;0,B27-1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C22" s="4">
+        <f>C27</f>
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4">
+        <f>40*C6+16*C7+34*J18</f>
+        <v>619285.92799999996</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.67</v>
+      </c>
+      <c r="G22" s="4">
+        <v>351.65</v>
+      </c>
+      <c r="H22" s="4">
+        <f>$I$2*G22</f>
+        <v>70.33</v>
+      </c>
+      <c r="I22">
+        <f>C22/F22</f>
+        <v>0.11859208412443391</v>
+      </c>
+      <c r="J22" s="27">
+        <f>E22+G22+H22</f>
+        <v>619707.90799999994</v>
+      </c>
+      <c r="K22" s="24"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="24">
+        <f>IF(B27&gt;0,B27-1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="4">
+        <f>C27</f>
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
+        <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
+        <v>151598.04399999999</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1758.23</v>
+      </c>
+      <c r="H23" s="4">
+        <f>$I$2*G23</f>
+        <v>351.64600000000002</v>
+      </c>
+      <c r="I23">
+        <f>C23/F23</f>
+        <v>0.60014781966001396</v>
+      </c>
+      <c r="J23" s="27">
+        <f>E23+G23+H23</f>
+        <v>153707.92000000001</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="40">
+        <v>1</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="39">
+        <f>(I22+I23)/G24</f>
+        <v>0.71873990378444785</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="39">
+        <f>I24*G24</f>
+        <v>0.71873990378444785</v>
+      </c>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="12">
+        <v>4</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="24">
+        <f>J22+J23</f>
+        <v>773415.82799999998</v>
+      </c>
+      <c r="F27" s="24">
+        <f>C27</f>
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="G27" s="24">
+        <v>12500</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27">
+        <f>C27/F27</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="27">
+        <f>E27+G27+H27</f>
+        <v>785915.82799999998</v>
+      </c>
+      <c r="K27" t="s">
+        <v>122</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="12">
+        <v>10</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="24">
+        <f>J27</f>
+        <v>785915.82799999998</v>
+      </c>
+      <c r="F30" s="24">
+        <v>4</v>
+      </c>
+      <c r="G30" s="42">
+        <f>518*B30*(128/(2^(B30-1)))</f>
+        <v>1295</v>
+      </c>
+      <c r="H30" s="24">
+        <f>G30*I2</f>
+        <v>259</v>
+      </c>
+      <c r="I30">
+        <f>C27/F30</f>
+        <v>4.9512195121951152E-2</v>
+      </c>
+      <c r="J30" s="27">
+        <f>E30+H30+G30</f>
+        <v>787469.82799999998</v>
+      </c>
+      <c r="K30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="24"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="12">
+        <f>790000+15000*B27</f>
+        <v>850000</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="24">
+        <f>24*C27</f>
+        <v>4.7531707317073106</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="27">
+        <f>(C34-J27)*C27</f>
+        <v>12691.792113170719</v>
+      </c>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="27">
+        <f>C36*24</f>
+        <v>304603.01071609725</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="12">
+        <v>318</v>
+      </c>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="24">
+        <v>2800</v>
+      </c>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="24">
+        <f>(0.5)^(B27+1)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="1">
+        <f>C40*C41*(1-C42)</f>
+        <v>862575</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="41">
+        <f>(C43-J30)*C27</f>
+        <v>14874.487722926813</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="41">
+        <f>C44*24</f>
+        <v>356987.70535024349</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M16:M17">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F5360406-8EFD-4FF6-B64C-F183DE818DE2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F5360406-8EFD-4FF6-B64C-F183DE818DE2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M16:M17</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="D3" s="4">
+        <f>20*C18</f>
+        <v>162.39999999999978</v>
+      </c>
+      <c r="E3" s="11">
+        <f>D3*C3</f>
+        <v>1705.1999999999978</v>
+      </c>
+      <c r="F3" s="11">
+        <f>E3*24</f>
+        <v>40924.799999999945</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>900</v>
+      </c>
+      <c r="D4" s="4">
+        <f>8*C18</f>
+        <v>64.959999999999908</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:E10" si="0">D4*C4</f>
+        <v>58463.99999999992</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" ref="F4:F10" si="1">E4*24</f>
+        <v>1403135.9999999981</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="K4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>18.5</v>
+      </c>
+      <c r="D5" s="4">
+        <f>10*C18</f>
+        <v>81.199999999999889</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>1502.199999999998</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="1"/>
+        <v>36052.799999999952</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24">
+        <f>IF(B22&gt;0,B22-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <f>3180*0.98</f>
+        <v>3116.4</v>
+      </c>
+      <c r="D6" s="4">
+        <f>40*C22</f>
+        <v>7.9219512195121844</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="0"/>
+        <v>24687.968780487772</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="1"/>
+        <v>592511.2507317065</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="12">
+        <f>9900*0.98</f>
+        <v>9702</v>
+      </c>
+      <c r="D7" s="4">
+        <f>16*C22+C23*6</f>
+        <v>4.3570731707317014</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="0"/>
+        <v>42272.32390243897</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="1"/>
+        <v>1014535.7736585352</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5570</v>
+      </c>
+      <c r="D8" s="4">
+        <f>2*C23</f>
+        <v>0.39609756097560922</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="0"/>
+        <v>2206.2634146341434</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="1"/>
+        <v>52950.321951219441</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="K8" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="12">
+        <v>545</v>
+      </c>
+      <c r="D9" s="4">
+        <f>10*C23</f>
+        <v>1.9804878048780461</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>1079.3658536585351</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>25904.780487804841</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1730</v>
+      </c>
+      <c r="D10" s="4">
+        <f>4*C23</f>
+        <v>0.79219512195121844</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="0"/>
+        <v>1370.4975609756079</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>32891.941463414594</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="27">
+        <f>SUM(E3:E10)</f>
+        <v>133287.81951219495</v>
+      </c>
+      <c r="F11" s="27">
+        <f>SUM(F3:F10)</f>
+        <v>3198907.6682926784</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="24"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="24">
+        <f>IF(B22&gt;0,B22-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C18" s="24">
+        <f>34*C22+7*C23</f>
+        <v>8.1199999999999886</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="24">
+        <f>20*C3+8*C4+10*C5</f>
+        <v>7595</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G18" s="24">
+        <v>1989.41</v>
+      </c>
+      <c r="H18" s="24">
+        <f>$I$2*G18</f>
+        <v>397.88200000000006</v>
+      </c>
+      <c r="I18">
+        <f>C18/F18</f>
+        <v>27.999999999999961</v>
+      </c>
+      <c r="J18" s="27">
+        <f>E18+G18+H18</f>
+        <v>9982.2919999999995</v>
+      </c>
+      <c r="K18" s="24"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="40">
+        <v>9</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="39">
+        <f>I18/G19</f>
+        <v>3.1111111111111067</v>
+      </c>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" s="39">
+        <f>I19*G19</f>
+        <v>27.999999999999961</v>
+      </c>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="24">
+        <f>IF(B27&gt;0,B27-1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C22" s="4">
+        <f>C27</f>
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4">
+        <f>40*C6+16*C7+34*J18</f>
+        <v>619285.92799999996</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.67</v>
+      </c>
+      <c r="G22" s="4">
+        <v>351.65</v>
+      </c>
+      <c r="H22" s="4">
+        <f>$I$2*G22</f>
+        <v>70.33</v>
+      </c>
+      <c r="I22">
+        <f>C22/F22</f>
+        <v>0.11859208412443391</v>
+      </c>
+      <c r="J22" s="27">
+        <f>E22+G22+H22</f>
+        <v>619707.90799999994</v>
+      </c>
+      <c r="K22" s="24"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="24">
+        <f>IF(B27&gt;0,B27-1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="4">
+        <f>C27</f>
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
+        <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
+        <v>151598.04399999999</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1758.23</v>
+      </c>
+      <c r="H23" s="4">
+        <f>$I$2*G23</f>
+        <v>351.64600000000002</v>
+      </c>
+      <c r="I23">
+        <f>C23/F23</f>
+        <v>0.60014781966001396</v>
+      </c>
+      <c r="J23" s="27">
+        <f>E23+G23+H23</f>
+        <v>153707.92000000001</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="40">
+        <v>1</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="39">
+        <f>(I22+I23)/G24</f>
+        <v>0.71873990378444785</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="39">
+        <f>I24*G24</f>
+        <v>0.71873990378444785</v>
+      </c>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="12">
+        <v>4</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0.19804878048780461</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="24">
+        <f>J22+J23</f>
+        <v>773415.82799999998</v>
+      </c>
+      <c r="F27" s="24">
+        <v>0.24</v>
+      </c>
+      <c r="G27" s="24">
+        <v>3170.85</v>
+      </c>
+      <c r="H27" s="24">
+        <f>$I$2*G27</f>
+        <v>634.17000000000007</v>
+      </c>
+      <c r="I27">
+        <f>C27/F27</f>
+        <v>0.82520325203251921</v>
+      </c>
+      <c r="J27" s="27">
+        <f>E27+G27+H27</f>
+        <v>777220.848</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="40">
+        <v>1</v>
+      </c>
+      <c r="H28" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="39">
+        <f>I27/G28</f>
+        <v>0.82520325203251921</v>
+      </c>
+      <c r="K28" t="s">
+        <v>128</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I29" s="39">
+        <f>I28*G28</f>
+        <v>0.82520325203251921</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="12">
+        <v>10</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="24">
+        <f>J27</f>
+        <v>777220.848</v>
+      </c>
+      <c r="F31" s="24">
+        <v>4</v>
+      </c>
+      <c r="G31" s="42">
+        <f>518*B31*(128/(2^(B31-1)))</f>
+        <v>1295</v>
+      </c>
+      <c r="H31" s="24">
+        <f>G31*I2</f>
+        <v>259</v>
+      </c>
+      <c r="I31">
+        <f>C27/F31</f>
+        <v>4.9512195121951152E-2</v>
+      </c>
+      <c r="J31" s="27">
+        <f>E31+G31+H31</f>
+        <v>778774.848</v>
+      </c>
+      <c r="K31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="12">
+        <f>790000+15000*B27</f>
+        <v>850000</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="24">
+        <f>24*C27</f>
+        <v>4.7531707317073106</v>
+      </c>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="27">
+        <f>(C35-J27)*C27</f>
+        <v>14413.822298536566</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="27">
+        <f>C37*24</f>
+        <v>345931.73516487761</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="12">
+        <v>318</v>
+      </c>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="24">
+        <v>2800</v>
+      </c>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="24">
+        <f>(0.5)^(B27+1)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="1">
+        <f>C41*C42*(1-C43)</f>
+        <v>862575</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="41">
+        <f>(C44-J31)*C27</f>
+        <v>16596.517908292662</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="41">
+        <f>C45*24</f>
+        <v>398316.4297990239</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M16:M17">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7B01C992-87E0-4469-A5D5-96D18C7DB011}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7B01C992-87E0-4469-A5D5-96D18C7DB011}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
           <xm:sqref>M16:M17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>

</xml_diff>

<commit_message>
Let's continue selling Rocket engines for a while
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="All of them" sheetId="12" r:id="rId1"/>
@@ -5632,8 +5632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6055,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="B14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6123,15 +6123,15 @@
       </c>
       <c r="D3" s="4">
         <f>20*C18</f>
-        <v>162.39999999999978</v>
+        <v>255.19999999999996</v>
       </c>
       <c r="E3" s="11">
         <f>D3*C3</f>
-        <v>1705.1999999999978</v>
+        <v>2679.5999999999995</v>
       </c>
       <c r="F3" s="11">
         <f>E3*24</f>
-        <v>40924.799999999945</v>
+        <v>64310.399999999987</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -6148,15 +6148,15 @@
       </c>
       <c r="D4" s="4">
         <f>8*C18</f>
-        <v>64.959999999999908</v>
+        <v>102.07999999999998</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" ref="E4:E10" si="0">D4*C4</f>
-        <v>58463.99999999992</v>
+        <v>91871.999999999985</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" ref="F4:F10" si="1">E4*24</f>
-        <v>1403135.9999999981</v>
+        <v>2204927.9999999995</v>
       </c>
       <c r="G4" s="4"/>
       <c r="K4" t="s">
@@ -6176,15 +6176,15 @@
       </c>
       <c r="D5" s="4">
         <f>10*C18</f>
-        <v>81.199999999999889</v>
+        <v>127.59999999999998</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>1502.199999999998</v>
+        <v>2360.5999999999995</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="1"/>
-        <v>36052.799999999952</v>
+        <v>56654.399999999987</v>
       </c>
       <c r="G5" s="4"/>
       <c r="K5" t="s">
@@ -6205,15 +6205,15 @@
       </c>
       <c r="D6" s="4">
         <f>40*C22</f>
-        <v>7.9219512195121844</v>
+        <v>12.448780487804875</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>24687.968780487772</v>
+        <v>38795.379512195112</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="1"/>
-        <v>592511.2507317065</v>
+        <v>931089.10829268268</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -6231,15 +6231,15 @@
       </c>
       <c r="D7" s="4">
         <f>16*C22+C23*6</f>
-        <v>4.3570731707317014</v>
+        <v>6.8468292682926819</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>42272.32390243897</v>
+        <v>66427.937560975595</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="1"/>
-        <v>1014535.7736585352</v>
+        <v>1594270.5014634142</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -6256,15 +6256,15 @@
       </c>
       <c r="D8" s="4">
         <f>2*C23</f>
-        <v>0.39609756097560922</v>
+        <v>0.62243902439024379</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>2206.2634146341434</v>
+        <v>3466.9853658536581</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="1"/>
-        <v>52950.321951219441</v>
+        <v>83207.648780487798</v>
       </c>
       <c r="G8" s="4"/>
       <c r="K8" s="39" t="s">
@@ -6287,15 +6287,15 @@
       </c>
       <c r="D9" s="4">
         <f>10*C23</f>
-        <v>1.9804878048780461</v>
+        <v>3.1121951219512187</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>1079.3658536585351</v>
+        <v>1696.1463414634143</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="1"/>
-        <v>25904.780487804841</v>
+        <v>40707.512195121941</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -6312,15 +6312,15 @@
       </c>
       <c r="D10" s="4">
         <f>4*C23</f>
-        <v>0.79219512195121844</v>
+        <v>1.2448780487804876</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>1370.4975609756079</v>
+        <v>2153.6390243902433</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
-        <v>32891.941463414594</v>
+        <v>51687.33658536584</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -6331,11 +6331,11 @@
       <c r="D11" s="4"/>
       <c r="E11" s="27">
         <f>SUM(E3:E10)</f>
-        <v>133287.81951219495</v>
+        <v>209452.287804878</v>
       </c>
       <c r="F11" s="27">
         <f>E11*24</f>
-        <v>3198907.6682926789</v>
+        <v>5026854.9073170722</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -6433,7 +6433,7 @@
       </c>
       <c r="C18" s="24">
         <f>34*C22+7*C23</f>
-        <v>8.1199999999999886</v>
+        <v>12.759999999999998</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>39</v>
@@ -6454,7 +6454,7 @@
       </c>
       <c r="I18">
         <f>C18/F18</f>
-        <v>27.999999999999961</v>
+        <v>43.999999999999993</v>
       </c>
       <c r="J18" s="27">
         <f>E18+G18+H18</f>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="I19" s="39">
         <f>I18/G19</f>
-        <v>2.5454545454545419</v>
+        <v>3.9999999999999996</v>
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="I20" s="39">
         <f>I19*G19</f>
-        <v>27.999999999999961</v>
+        <v>43.999999999999993</v>
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
@@ -6534,7 +6534,7 @@
       </c>
       <c r="C22" s="4">
         <f>C27</f>
-        <v>0.19804878048780461</v>
+        <v>0.31121951219512189</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>22</v>
@@ -6555,7 +6555,7 @@
       </c>
       <c r="I22">
         <f>C22/F22</f>
-        <v>0.11859208412443391</v>
+        <v>0.18635898933839634</v>
       </c>
       <c r="J22" s="27">
         <f>E22+G22+H22</f>
@@ -6575,7 +6575,7 @@
       </c>
       <c r="C23" s="4">
         <f>C27</f>
-        <v>0.19804878048780461</v>
+        <v>0.31121951219512189</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>25</v>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="I23">
         <f>C23/F23</f>
-        <v>0.60014781966001396</v>
+        <v>0.94308943089430874</v>
       </c>
       <c r="J23" s="27">
         <f>E23+G23+H23</f>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="I24" s="39">
         <f>(I22+I23)/G24</f>
-        <v>0.71873990378444785</v>
+        <v>1.1294484202327051</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
@@ -6643,7 +6643,7 @@
       </c>
       <c r="I25" s="39">
         <f>I24*G24</f>
-        <v>0.71873990378444785</v>
+        <v>1.1294484202327051</v>
       </c>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
@@ -6674,7 +6674,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="12">
-        <v>0.19804878048780461</v>
+        <v>0.31121951219512189</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="24">
@@ -6683,7 +6683,7 @@
       </c>
       <c r="F27" s="24">
         <f>C27</f>
-        <v>0.19804878048780461</v>
+        <v>0.31121951219512189</v>
       </c>
       <c r="G27" s="24">
         <v>12500</v>
@@ -6761,7 +6761,7 @@
       </c>
       <c r="I30">
         <f>C27/F30</f>
-        <v>4.9512195121951152E-2</v>
+        <v>7.7804878048780474E-2</v>
       </c>
       <c r="J30" s="27">
         <f>E30+H30+G30</f>
@@ -6788,7 +6788,7 @@
       </c>
       <c r="I31" s="39">
         <f>(I30)/G31</f>
-        <v>4.9512195121951152E-2</v>
+        <v>7.7804878048780474E-2</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="I32" s="39">
         <f>I31*G31</f>
-        <v>4.9512195121951152E-2</v>
+        <v>7.7804878048780474E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -6839,7 +6839,7 @@
       </c>
       <c r="C35" s="24">
         <f>24*C27</f>
-        <v>4.7531707317073106</v>
+        <v>7.4692682926829255</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -6852,7 +6852,7 @@
       </c>
       <c r="C36" s="27">
         <f>(C34-J27)*C27</f>
-        <v>12691.792113170719</v>
+        <v>19944.244749268295</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="C37" s="27">
         <f>C36*24</f>
-        <v>304603.01071609725</v>
+        <v>478661.87398243905</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="C44" s="41">
         <f>(C43-J30)*C27</f>
-        <v>14874.487722926813</v>
+        <v>23374.194993170735</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -6944,7 +6944,7 @@
       </c>
       <c r="C45" s="41">
         <f>C44*24</f>
-        <v>356987.70535024349</v>
+        <v>560980.67983609764</v>
       </c>
     </row>
   </sheetData>
@@ -6988,8 +6988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7055,15 +7055,15 @@
       </c>
       <c r="D3" s="4">
         <f>20*C18</f>
-        <v>162.39999999999978</v>
+        <v>232.00000000000003</v>
       </c>
       <c r="E3" s="11">
         <f>D3*C3</f>
-        <v>1705.1999999999978</v>
+        <v>2436.0000000000005</v>
       </c>
       <c r="F3" s="11">
         <f>E3*24</f>
-        <v>40924.799999999945</v>
+        <v>58464.000000000015</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -7076,19 +7076,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="12">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="D4" s="4">
         <f>8*C18</f>
-        <v>64.959999999999908</v>
+        <v>92.800000000000011</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" ref="E4:E10" si="0">D4*C4</f>
-        <v>71455.999999999898</v>
+        <v>83520.000000000015</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" ref="F4:F10" si="1">E4*24</f>
-        <v>1714943.9999999977</v>
+        <v>2004480.0000000005</v>
       </c>
       <c r="G4" s="4"/>
       <c r="K4" t="s">
@@ -7108,15 +7108,15 @@
       </c>
       <c r="D5" s="4">
         <f>10*C18</f>
-        <v>81.199999999999889</v>
+        <v>116.00000000000001</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>1502.199999999998</v>
+        <v>2146.0000000000005</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="1"/>
-        <v>36052.799999999952</v>
+        <v>51504.000000000015</v>
       </c>
       <c r="G5" s="4"/>
       <c r="K5" t="s">
@@ -7137,15 +7137,15 @@
       </c>
       <c r="D6" s="4">
         <f>40*C22</f>
-        <v>7.9219512195121844</v>
+        <v>11.317073170731708</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>24687.968780487772</v>
+        <v>35268.526829268296</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="1"/>
-        <v>592511.2507317065</v>
+        <v>846444.64390243916</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -7163,15 +7163,15 @@
       </c>
       <c r="D7" s="4">
         <f>16*C22+C23*6</f>
-        <v>4.3570731707317014</v>
+        <v>6.2243902439024392</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>42272.32390243897</v>
+        <v>60389.034146341466</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="1"/>
-        <v>1014535.7736585352</v>
+        <v>1449336.8195121952</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -7188,15 +7188,15 @@
       </c>
       <c r="D8" s="4">
         <f>2*C23</f>
-        <v>0.39609756097560922</v>
+        <v>0.56585365853658542</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>2206.2634146341434</v>
+        <v>3151.8048780487807</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="1"/>
-        <v>52950.321951219441</v>
+        <v>75643.317073170736</v>
       </c>
       <c r="G8" s="4"/>
       <c r="K8" s="39" t="s">
@@ -7219,15 +7219,15 @@
       </c>
       <c r="D9" s="4">
         <f>10*C23</f>
-        <v>1.9804878048780461</v>
+        <v>2.8292682926829271</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>1079.3658536585351</v>
+        <v>1541.9512195121954</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="1"/>
-        <v>25904.780487804841</v>
+        <v>37006.829268292691</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -7244,15 +7244,15 @@
       </c>
       <c r="D10" s="4">
         <f>4*C23</f>
-        <v>0.79219512195121844</v>
+        <v>1.1317073170731708</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>1370.4975609756079</v>
+        <v>1957.8536585365855</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
-        <v>32891.941463414594</v>
+        <v>46988.487804878052</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -7263,11 +7263,11 @@
       <c r="D11" s="4"/>
       <c r="E11" s="27">
         <f>SUM(E3:E10)</f>
-        <v>146279.8195121949</v>
+        <v>190411.17073170736</v>
       </c>
       <c r="F11" s="27">
         <f>SUM(F3:F10)</f>
-        <v>3510715.6682926784</v>
+        <v>4569868.0975609766</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -7365,14 +7365,14 @@
       </c>
       <c r="C18" s="24">
         <f>34*C22+7*C23</f>
-        <v>8.1199999999999886</v>
+        <v>11.600000000000001</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="24">
         <f>20*C3+8*C4+10*C5</f>
-        <v>9195</v>
+        <v>7595</v>
       </c>
       <c r="F18" s="24">
         <v>0.28999999999999998</v>
@@ -7386,11 +7386,11 @@
       </c>
       <c r="I18">
         <f>C18/F18</f>
-        <v>27.999999999999961</v>
+        <v>40.000000000000007</v>
       </c>
       <c r="J18" s="27">
         <f>E18+G18+H18</f>
-        <v>11582.291999999999</v>
+        <v>9982.2919999999995</v>
       </c>
       <c r="K18" s="24"/>
       <c r="L18" s="4"/>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="I19" s="39">
         <f>I18/G19</f>
-        <v>2.7999999999999963</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
@@ -7433,7 +7433,7 @@
       </c>
       <c r="I20" s="39">
         <f>I19*G19</f>
-        <v>27.999999999999964</v>
+        <v>40.000000000000007</v>
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
@@ -7466,14 +7466,14 @@
       </c>
       <c r="C22" s="4">
         <f>C27</f>
-        <v>0.19804878048780461</v>
+        <v>0.28292682926829271</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="4">
         <f>40*C6+16*C7+34*J18</f>
-        <v>673685.92799999996</v>
+        <v>619285.92799999996</v>
       </c>
       <c r="F22" s="4">
         <v>1.67</v>
@@ -7487,11 +7487,11 @@
       </c>
       <c r="I22">
         <f>C22/F22</f>
-        <v>0.11859208412443391</v>
+        <v>0.16941726303490581</v>
       </c>
       <c r="J22" s="27">
         <f>E22+G22+H22</f>
-        <v>674107.90799999994</v>
+        <v>619707.90799999994</v>
       </c>
       <c r="K22" s="24"/>
       <c r="L22" s="4"/>
@@ -7507,14 +7507,14 @@
       </c>
       <c r="C23" s="4">
         <f>C27</f>
-        <v>0.19804878048780461</v>
+        <v>0.28292682926829271</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="4">
         <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
-        <v>162798.04399999999</v>
+        <v>151598.04399999999</v>
       </c>
       <c r="F23" s="4">
         <v>0.33</v>
@@ -7528,11 +7528,11 @@
       </c>
       <c r="I23">
         <f>C23/F23</f>
-        <v>0.60014781966001396</v>
+        <v>0.85735402808573546</v>
       </c>
       <c r="J23" s="27">
         <f>E23+G23+H23</f>
-        <v>164907.92000000001</v>
+        <v>153707.92000000001</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="4"/>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="I24" s="39">
         <f>(I22+I23)/G24</f>
-        <v>0.71873990378444785</v>
+        <v>1.0267712911206412</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
@@ -7575,7 +7575,7 @@
       </c>
       <c r="I25" s="39">
         <f>I24*G24</f>
-        <v>0.71873990378444785</v>
+        <v>1.0267712911206412</v>
       </c>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
@@ -7606,14 +7606,14 @@
         <v>4</v>
       </c>
       <c r="C27" s="12">
-        <v>0.19804878048780461</v>
+        <v>0.28292682926829271</v>
       </c>
       <c r="D27" s="28" t="s">
         <v>48</v>
       </c>
       <c r="E27" s="24">
         <f>J22+J23</f>
-        <v>839015.82799999998</v>
+        <v>773415.82799999998</v>
       </c>
       <c r="F27" s="24">
         <v>0.24</v>
@@ -7627,11 +7627,11 @@
       </c>
       <c r="I27">
         <f>C27/F27</f>
-        <v>0.82520325203251921</v>
+        <v>1.1788617886178863</v>
       </c>
       <c r="J27" s="27">
         <f>E27+G27+H27</f>
-        <v>842820.848</v>
+        <v>777220.848</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -7653,7 +7653,7 @@
       </c>
       <c r="I28" s="39">
         <f>I27/G28</f>
-        <v>0.82520325203251921</v>
+        <v>1.1788617886178863</v>
       </c>
       <c r="K28" t="s">
         <v>127</v>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="I29" s="39">
         <f>I28*G28</f>
-        <v>0.82520325203251921</v>
+        <v>1.1788617886178863</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -7709,7 +7709,7 @@
       </c>
       <c r="E31" s="24">
         <f>J27</f>
-        <v>842820.848</v>
+        <v>777220.848</v>
       </c>
       <c r="F31" s="24">
         <v>4</v>
@@ -7724,11 +7724,11 @@
       </c>
       <c r="I31">
         <f>C27/F31</f>
-        <v>4.9512195121951152E-2</v>
+        <v>7.0731707317073178E-2</v>
       </c>
       <c r="J31" s="27">
         <f>E31+G31+H31</f>
-        <v>844374.848</v>
+        <v>778774.848</v>
       </c>
       <c r="K31" t="s">
         <v>126</v>
@@ -7751,7 +7751,7 @@
       </c>
       <c r="I32" s="39">
         <f>(I31)/G32</f>
-        <v>4.9512195121951152E-2</v>
+        <v>7.0731707317073178E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -7766,7 +7766,7 @@
       </c>
       <c r="I33" s="39">
         <f>I32*G32</f>
-        <v>4.9512195121951152E-2</v>
+        <v>7.0731707317073178E-2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -7802,7 +7802,7 @@
       </c>
       <c r="C36" s="24">
         <f>24*C27</f>
-        <v>4.7531707317073106</v>
+        <v>6.7902439024390251</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -7815,7 +7815,7 @@
       </c>
       <c r="C37" s="27">
         <f>(C35-J27)*C27</f>
-        <v>1421.8222985365837</v>
+        <v>20591.174712195123</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -7828,7 +7828,7 @@
       </c>
       <c r="C38" s="27">
         <f>C37*24</f>
-        <v>34123.73516487801</v>
+        <v>494188.19309268298</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -7898,7 +7898,7 @@
       </c>
       <c r="C45" s="41">
         <f>(C44-J31)*C27</f>
-        <v>3604.5179082926784</v>
+        <v>23709.31129756098</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -7907,7 +7907,7 @@
       </c>
       <c r="C46" s="41">
         <f>C45*24</f>
-        <v>86508.429799024278</v>
+        <v>569023.47114146349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Not so expensive to rent Launchpads
a little bit expensive to rent VIFs
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -20,7 +20,8 @@
     <sheet name="SORs" sheetId="5" r:id="rId6"/>
     <sheet name="Rocket production" sheetId="13" r:id="rId7"/>
     <sheet name="Production Plans second stage" sheetId="15" r:id="rId8"/>
-    <sheet name="Production Plans final stage" sheetId="14" r:id="rId9"/>
+    <sheet name="Production Plans third stage" sheetId="16" r:id="rId9"/>
+    <sheet name="Production Plans final stage" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="146">
   <si>
     <t>Carbon composite</t>
   </si>
@@ -394,12 +395,6 @@
     <t>BFR with VIF rent</t>
   </si>
   <si>
-    <t>For the first stage we only pretend to sell BFRs</t>
-  </si>
-  <si>
-    <t>For the second stage we pretend to build a high q launchpad and sell ASR</t>
-  </si>
-  <si>
     <t>REQUIRED CASH PER HOUR</t>
   </si>
   <si>
@@ -409,12 +404,6 @@
     <t>PRODUCED UNITS PER HOUR</t>
   </si>
   <si>
-    <t>Assuming we will prefer to launch our BFRs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assuming we can produce our own high quality BFRs. </t>
-  </si>
-  <si>
     <t>UNITS PER HOUR PER LEVEL</t>
   </si>
   <si>
@@ -431,13 +420,65 @@
   </si>
   <si>
     <t>NEEDS PER DAY</t>
+  </si>
+  <si>
+    <t>We will launch our own BFRs on our own Launchpads</t>
+  </si>
+  <si>
+    <t>We will produce our own high q BFRs</t>
+  </si>
+  <si>
+    <t>We will pay someone to build our BFRs</t>
+  </si>
+  <si>
+    <t>We will launch our own BFRs</t>
+  </si>
+  <si>
+    <t>BFR costs of launching:</t>
+  </si>
+  <si>
+    <t>AMOUNT RECEIVED AFTER COMMISION</t>
+  </si>
+  <si>
+    <t>(Assuming our partner is SOR06TURK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No commision ratio </t>
+  </si>
+  <si>
+    <t>Cost per ASR</t>
+  </si>
+  <si>
+    <t>Real cost if launched by me</t>
+  </si>
+  <si>
+    <t>Cost of launching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio with commision </t>
+  </si>
+  <si>
+    <t>Real probability of failure</t>
+  </si>
+  <si>
+    <t>Paid probability of failure</t>
+  </si>
+  <si>
+    <t>For this to be profitable we should have a lvl 10 launchpad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Or we should pay the rent of it. </t>
+  </si>
+  <si>
+    <t>We will also pay someoune to launch our BFRs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -674,7 +715,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,6 +760,7 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -1946,6 +1988,1005 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M46"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="14">
+        <f>SUM(I20,I25,I29,I33)/170</f>
+        <v>0.27353579796703847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="D3" s="4">
+        <f>20*C18</f>
+        <v>255.184</v>
+      </c>
+      <c r="E3">
+        <f>D3*24</f>
+        <v>6124.4160000000002</v>
+      </c>
+      <c r="F3" s="41">
+        <f t="shared" ref="F3:F10" si="0">D3*C3</f>
+        <v>2679.4319999999998</v>
+      </c>
+      <c r="G3" s="41">
+        <f>F3*24</f>
+        <v>64306.367999999995</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>900</v>
+      </c>
+      <c r="D4" s="4">
+        <f>8*C18</f>
+        <v>102.0736</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="1">D4*24</f>
+        <v>2449.7664</v>
+      </c>
+      <c r="F4" s="41">
+        <f t="shared" si="0"/>
+        <v>91866.240000000005</v>
+      </c>
+      <c r="G4" s="41">
+        <f t="shared" ref="G4:G10" si="2">F4*24</f>
+        <v>2204789.7600000002</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f>IF(B18&gt;0,B18-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>18.5</v>
+      </c>
+      <c r="D5" s="4">
+        <f>10*C18</f>
+        <v>127.592</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>3062.2080000000001</v>
+      </c>
+      <c r="F5" s="41">
+        <f t="shared" si="0"/>
+        <v>2360.4519999999998</v>
+      </c>
+      <c r="G5" s="41">
+        <f t="shared" si="2"/>
+        <v>56650.847999999998</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24">
+        <f>IF(B22&gt;0,B22-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <f>3180*0.98</f>
+        <v>3116.4</v>
+      </c>
+      <c r="D6" s="4">
+        <f>40*C22</f>
+        <v>12.447999999999999</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>298.75199999999995</v>
+      </c>
+      <c r="F6" s="41">
+        <f t="shared" si="0"/>
+        <v>38792.947199999995</v>
+      </c>
+      <c r="G6" s="41">
+        <f t="shared" si="2"/>
+        <v>931030.73279999988</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="12">
+        <f>9900*0.98</f>
+        <v>9702</v>
+      </c>
+      <c r="D7" s="4">
+        <f>16*C22+C23*6</f>
+        <v>6.8463999999999992</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>164.31359999999998</v>
+      </c>
+      <c r="F7" s="41">
+        <f t="shared" si="0"/>
+        <v>66423.772799999992</v>
+      </c>
+      <c r="G7" s="41">
+        <f t="shared" si="2"/>
+        <v>1594170.5471999999</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5570</v>
+      </c>
+      <c r="D8" s="4">
+        <f>2*C23</f>
+        <v>0.62239999999999995</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>14.9376</v>
+      </c>
+      <c r="F8" s="41">
+        <f t="shared" si="0"/>
+        <v>3466.7679999999996</v>
+      </c>
+      <c r="G8" s="41">
+        <f t="shared" si="2"/>
+        <v>83202.431999999986</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="L8" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="12">
+        <v>545</v>
+      </c>
+      <c r="D9" s="4">
+        <f>10*C23</f>
+        <v>3.1119999999999997</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>74.687999999999988</v>
+      </c>
+      <c r="F9" s="41">
+        <f t="shared" si="0"/>
+        <v>1696.0399999999997</v>
+      </c>
+      <c r="G9" s="41">
+        <f t="shared" si="2"/>
+        <v>40704.959999999992</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="24">
+        <f>IF(B23&gt;0,B23-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1730</v>
+      </c>
+      <c r="D10" s="4">
+        <f>4*C23</f>
+        <v>1.2447999999999999</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>29.8752</v>
+      </c>
+      <c r="F10" s="41">
+        <f t="shared" si="0"/>
+        <v>2153.5039999999999</v>
+      </c>
+      <c r="G10" s="41">
+        <f t="shared" si="2"/>
+        <v>51684.095999999998</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="F11" s="42">
+        <f>SUM(F3:F10)</f>
+        <v>209439.15599999999</v>
+      </c>
+      <c r="G11" s="42">
+        <f>SUM(G3:G10)</f>
+        <v>5026539.743999999</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="24"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="24">
+        <f>IF(B22&gt;0,B22-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C18" s="24">
+        <f>34*C22+7*C23</f>
+        <v>12.7592</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="24">
+        <f>20*C3+8*C4+10*C5</f>
+        <v>7595</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G18" s="24">
+        <v>1989.41</v>
+      </c>
+      <c r="H18" s="24">
+        <f>$J$2*G18</f>
+        <v>544.174851833606</v>
+      </c>
+      <c r="I18">
+        <f>C18/F18</f>
+        <v>43.997241379310346</v>
+      </c>
+      <c r="J18" s="42">
+        <f>E18+G18+H18</f>
+        <v>10128.584851833606</v>
+      </c>
+      <c r="K18" s="24"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="39">
+        <v>10</v>
+      </c>
+      <c r="H19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" s="38">
+        <f>I18/G19</f>
+        <v>4.3997241379310346</v>
+      </c>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="38">
+        <f>I19*G19</f>
+        <v>43.997241379310346</v>
+      </c>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="24">
+        <f>IF(B27&gt;0,B27-1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C22" s="4">
+        <f>C27</f>
+        <v>0.31119999999999998</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4">
+        <f>40*C6+16*C7+34*J18</f>
+        <v>624259.88496234268</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.67</v>
+      </c>
+      <c r="G22" s="4">
+        <v>351.65</v>
+      </c>
+      <c r="H22" s="4">
+        <f>$J$2*G22</f>
+        <v>96.188863355109078</v>
+      </c>
+      <c r="I22">
+        <f>C22/F22</f>
+        <v>0.18634730538922156</v>
+      </c>
+      <c r="J22" s="42">
+        <f>E22+G22+H22</f>
+        <v>624707.72382569779</v>
+      </c>
+      <c r="K22" s="24"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="24">
+        <f>IF(B27&gt;0,B27-1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="4">
+        <f>C27</f>
+        <v>0.31119999999999998</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
+        <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
+        <v>152622.09396283524</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1758.23</v>
+      </c>
+      <c r="H23" s="4">
+        <f>$J$2*G23</f>
+        <v>480.93884605958607</v>
+      </c>
+      <c r="I23">
+        <f>C23/F23</f>
+        <v>0.94303030303030289</v>
+      </c>
+      <c r="J23" s="42">
+        <f>E23+G23+H23</f>
+        <v>154861.26280889483</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="39">
+        <v>1</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="38">
+        <f>(I22+I23)/G24</f>
+        <v>1.1293776084195244</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="38">
+        <f>I24*G24</f>
+        <v>1.1293776084195244</v>
+      </c>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="12">
+        <v>4</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0.31119999999999998</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="24">
+        <f>J22+J23</f>
+        <v>779568.98663459264</v>
+      </c>
+      <c r="F27" s="24">
+        <v>0.24</v>
+      </c>
+      <c r="G27" s="24">
+        <v>3170.85</v>
+      </c>
+      <c r="H27" s="24">
+        <f>$J$2*G27</f>
+        <v>867.34098498378387</v>
+      </c>
+      <c r="I27">
+        <f>C27/F27</f>
+        <v>1.2966666666666666</v>
+      </c>
+      <c r="J27" s="42">
+        <f>E27+G27+H27</f>
+        <v>783607.17761957645</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="39">
+        <v>1</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="38">
+        <f>I27/G28</f>
+        <v>1.2966666666666666</v>
+      </c>
+      <c r="K28" t="s">
+        <v>130</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="38">
+        <f>I28*G28</f>
+        <v>1.2966666666666666</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="12">
+        <v>10</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="24">
+        <f>J27</f>
+        <v>783607.17761957645</v>
+      </c>
+      <c r="F31" s="24">
+        <v>4</v>
+      </c>
+      <c r="G31" s="40">
+        <f>518*B31*(128/(2^(B31-1)))</f>
+        <v>1295</v>
+      </c>
+      <c r="H31" s="24">
+        <f>G31*J2</f>
+        <v>354.22885836731484</v>
+      </c>
+      <c r="I31">
+        <f>C27/F31</f>
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="J31" s="42">
+        <f>E31+G31+H31</f>
+        <v>785256.40647794376</v>
+      </c>
+      <c r="K31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="39">
+        <v>1</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I32" s="38">
+        <f>(I31)/G32</f>
+        <v>7.7799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="38">
+        <f>I32*G32</f>
+        <v>7.7799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="12">
+        <f>790000+15000*B27</f>
+        <v>850000</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="24">
+        <f>24*C27</f>
+        <v>7.4687999999999999</v>
+      </c>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="42">
+        <f>(C35-J27)*C27</f>
+        <v>20661.446324787805</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="42">
+        <f>C37*24</f>
+        <v>495874.71179490734</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="12">
+        <v>307</v>
+      </c>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="24">
+        <v>2800</v>
+      </c>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="24">
+        <f>(0.5)^(B27+1)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="1">
+        <f>C41*C42*(1-C43)</f>
+        <v>832737.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="43">
+        <f>(C44-J31)*C27</f>
+        <v>14776.1163040639</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="43">
+        <f>C45*24</f>
+        <v>354626.79129753361</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M16:M17">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7B01C992-87E0-4469-A5D5-96D18C7DB011}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7B01C992-87E0-4469-A5D5-96D18C7DB011}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M16:M17</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K41"/>
@@ -5648,7 +6689,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5686,16 +6727,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="13" t="s">
@@ -5801,7 +6842,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -6007,7 +7048,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C18" s="24">
         <f>C13*24</f>
@@ -6093,10 +7134,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,11 +7147,11 @@
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="75.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6134,24 +7175,24 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="14">
-        <f>SUM(I20,I25,I32)/170</f>
-        <v>0.26592501940165575</v>
+        <f>SUM(I20,I25)/170</f>
+        <v>0.30166743596412232</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6163,23 +7204,23 @@
         <v>1</v>
       </c>
       <c r="C3" s="12">
-        <v>10.5</v>
+        <v>10.9</v>
       </c>
       <c r="D3" s="4">
         <f>20*C18</f>
-        <v>255.19999999999996</v>
+        <v>289.99999999999994</v>
       </c>
       <c r="E3">
         <f>D3*24</f>
-        <v>6124.7999999999993</v>
+        <v>6959.9999999999982</v>
       </c>
       <c r="F3" s="41">
         <f t="shared" ref="F3:F10" si="0">D3*C3</f>
-        <v>2679.5999999999995</v>
+        <v>3160.9999999999995</v>
       </c>
       <c r="G3" s="41">
         <f>F3*24</f>
-        <v>64310.399999999987</v>
+        <v>75863.999999999985</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -6192,23 +7233,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="12">
-        <v>900</v>
+        <v>820</v>
       </c>
       <c r="D4" s="4">
         <f>8*C18</f>
-        <v>102.07999999999998</v>
+        <v>115.99999999999997</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E10" si="1">D4*24</f>
-        <v>2449.9199999999996</v>
+        <v>2783.9999999999991</v>
       </c>
       <c r="F4" s="41">
         <f t="shared" si="0"/>
-        <v>91871.999999999985</v>
+        <v>95119.999999999971</v>
       </c>
       <c r="G4" s="41">
         <f t="shared" ref="G4:G10" si="2">F4*24</f>
-        <v>2204927.9999999995</v>
+        <v>2282879.9999999991</v>
       </c>
       <c r="H4" s="4"/>
       <c r="L4" t="s">
@@ -6224,23 +7265,23 @@
         <v>1</v>
       </c>
       <c r="C5" s="12">
-        <v>18.5</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4">
         <f>10*C18</f>
-        <v>127.59999999999998</v>
+        <v>144.99999999999997</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>3062.3999999999996</v>
+        <v>3479.9999999999991</v>
       </c>
       <c r="F5" s="41">
         <f t="shared" si="0"/>
-        <v>2360.5999999999995</v>
+        <v>2754.9999999999995</v>
       </c>
       <c r="G5" s="41">
         <f t="shared" si="2"/>
-        <v>56654.399999999987</v>
+        <v>66119.999999999985</v>
       </c>
       <c r="H5" s="4"/>
       <c r="L5" t="s">
@@ -6256,24 +7297,23 @@
         <v>2</v>
       </c>
       <c r="C6" s="12">
-        <f>3180*0.98</f>
-        <v>3116.4</v>
+        <v>2700</v>
       </c>
       <c r="D6" s="4">
         <f>40*C22</f>
-        <v>12.448780487804875</v>
+        <v>14.146341463414631</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>298.770731707317</v>
+        <v>339.51219512195115</v>
       </c>
       <c r="F6" s="41">
         <f t="shared" si="0"/>
-        <v>38795.379512195112</v>
+        <v>38195.121951219502</v>
       </c>
       <c r="G6" s="41">
         <f t="shared" si="2"/>
-        <v>931089.10829268268</v>
+        <v>916682.92682926799</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -6286,24 +7326,23 @@
         <v>2</v>
       </c>
       <c r="C7" s="12">
-        <f>9900*0.98</f>
-        <v>9702</v>
+        <v>8800</v>
       </c>
       <c r="D7" s="4">
         <f>16*C22+C23*6</f>
-        <v>6.8468292682926819</v>
+        <v>7.7804878048780477</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>164.32390243902438</v>
+        <v>186.73170731707313</v>
       </c>
       <c r="F7" s="41">
         <f t="shared" si="0"/>
-        <v>66427.937560975595</v>
+        <v>68468.292682926825</v>
       </c>
       <c r="G7" s="41">
         <f t="shared" si="2"/>
-        <v>1594270.5014634142</v>
+        <v>1643239.0243902439</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -6320,19 +7359,19 @@
       </c>
       <c r="D8" s="4">
         <f>2*C23</f>
-        <v>0.62243902439024379</v>
+        <v>0.70731707317073156</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>14.938536585365851</v>
+        <v>16.975609756097558</v>
       </c>
       <c r="F8" s="41">
         <f t="shared" si="0"/>
-        <v>3466.9853658536581</v>
+        <v>3939.7560975609749</v>
       </c>
       <c r="G8" s="41">
         <f t="shared" si="2"/>
-        <v>83207.648780487798</v>
+        <v>94554.146341463405</v>
       </c>
       <c r="H8" s="4"/>
       <c r="L8" s="38" t="s">
@@ -6355,19 +7394,19 @@
       </c>
       <c r="D9" s="4">
         <f>10*C23</f>
-        <v>3.1121951219512187</v>
+        <v>3.5365853658536577</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>74.692682926829249</v>
+        <v>84.878048780487788</v>
       </c>
       <c r="F9" s="41">
         <f t="shared" si="0"/>
-        <v>1696.1463414634143</v>
+        <v>1927.4390243902435</v>
       </c>
       <c r="G9" s="41">
         <f t="shared" si="2"/>
-        <v>40707.512195121941</v>
+        <v>46258.536585365844</v>
       </c>
       <c r="H9" s="4"/>
     </row>
@@ -6384,19 +7423,19 @@
       </c>
       <c r="D10" s="4">
         <f>4*C23</f>
-        <v>1.2448780487804876</v>
+        <v>1.4146341463414631</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>29.877073170731702</v>
+        <v>33.951219512195117</v>
       </c>
       <c r="F10" s="41">
         <f t="shared" si="0"/>
-        <v>2153.6390243902433</v>
+        <v>2447.3170731707314</v>
       </c>
       <c r="G10" s="41">
         <f t="shared" si="2"/>
-        <v>51687.33658536584</v>
+        <v>58735.609756097554</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -6407,11 +7446,11 @@
       <c r="D11" s="4"/>
       <c r="F11" s="42">
         <f>SUM(F3:F10)</f>
-        <v>209452.287804878</v>
+        <v>216013.92682926828</v>
       </c>
       <c r="G11" s="42">
         <f>F11*24</f>
-        <v>5026854.9073170722</v>
+        <v>5184334.2439024393</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -6456,7 +7495,7 @@
         <v>100</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>4</v>
@@ -6465,7 +7504,7 @@
         <v>84</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>7</v>
@@ -6509,14 +7548,14 @@
       </c>
       <c r="C18" s="24">
         <f>34*C22+7*C23</f>
-        <v>12.759999999999998</v>
+        <v>14.499999999999996</v>
       </c>
       <c r="D18" s="27" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="24">
         <f>20*C3+8*C4+10*C5</f>
-        <v>7595</v>
+        <v>6968</v>
       </c>
       <c r="F18" s="24">
         <v>0.28999999999999998</v>
@@ -6526,15 +7565,15 @@
       </c>
       <c r="H18" s="24">
         <f>$J$2*G18</f>
-        <v>529.03389284784794</v>
+        <v>600.14021378138466</v>
       </c>
       <c r="I18">
         <f>C18/F18</f>
-        <v>43.999999999999993</v>
+        <v>49.999999999999993</v>
       </c>
       <c r="J18" s="42">
         <f>E18+G18+H18</f>
-        <v>10113.443892847848</v>
+        <v>9557.5502137813837</v>
       </c>
       <c r="K18" s="24"/>
       <c r="L18" s="4"/>
@@ -6550,14 +7589,14 @@
         <v>101</v>
       </c>
       <c r="G19" s="39">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H19" s="38" t="s">
         <v>102</v>
       </c>
       <c r="I19" s="38">
         <f>I18/G19</f>
-        <v>3.9999999999999996</v>
+        <v>4.1666666666666661</v>
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
@@ -6577,7 +7616,7 @@
       </c>
       <c r="I20" s="38">
         <f>I19*G19</f>
-        <v>43.999999999999993</v>
+        <v>49.999999999999993</v>
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
@@ -6610,14 +7649,14 @@
       </c>
       <c r="C22" s="4">
         <f>C27</f>
-        <v>0.31121951219512189</v>
+        <v>0.35365853658536578</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="4">
         <f>40*C6+16*C7+34*J18</f>
-        <v>623745.09235682688</v>
+        <v>573756.70726856706</v>
       </c>
       <c r="F22" s="4">
         <v>1.67</v>
@@ -6627,15 +7666,15 @@
       </c>
       <c r="H22" s="4">
         <f>$J$2*G22</f>
-        <v>93.512533072592234</v>
+        <v>106.08135385678361</v>
       </c>
       <c r="I22">
         <f>C22/F22</f>
-        <v>0.18635898933839634</v>
+        <v>0.2117715787936322</v>
       </c>
       <c r="J22" s="42">
         <f>E22+G22+H22</f>
-        <v>624190.25488989952</v>
+        <v>574214.43862242391</v>
       </c>
       <c r="K22" s="24"/>
       <c r="L22" s="4"/>
@@ -6651,14 +7690,14 @@
       </c>
       <c r="C23" s="4">
         <f>C27</f>
-        <v>0.31121951219512189</v>
+        <v>0.35365853658536578</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="4">
         <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
-        <v>152516.10724993492</v>
+        <v>143212.8514964697</v>
       </c>
       <c r="F23" s="4">
         <v>0.33</v>
@@ -6668,15 +7707,15 @@
       </c>
       <c r="H23" s="4">
         <f>$J$2*G23</f>
-        <v>467.55734686257318</v>
+        <v>530.40073593519878</v>
       </c>
       <c r="I23">
         <f>C23/F23</f>
-        <v>0.94308943089430874</v>
+        <v>1.0716925351071689</v>
       </c>
       <c r="J23" s="42">
         <f>E23+G23+H23</f>
-        <v>154741.8945967975</v>
+        <v>145501.4822324049</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="4"/>
@@ -6699,7 +7738,7 @@
       </c>
       <c r="I24" s="38">
         <f>(I22+I23)/G24</f>
-        <v>1.1294484202327051</v>
+        <v>1.2834641139008012</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
@@ -6719,7 +7758,7 @@
       </c>
       <c r="I25" s="38">
         <f>I24*G24</f>
-        <v>1.1294484202327051</v>
+        <v>1.2834641139008012</v>
       </c>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
@@ -6750,16 +7789,16 @@
         <v>4</v>
       </c>
       <c r="C27" s="12">
-        <v>0.31121951219512189</v>
+        <v>0.35365853658536578</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="24">
         <f>J22+J23</f>
-        <v>778932.14948669705</v>
+        <v>719715.92085482879</v>
       </c>
       <c r="F27" s="24">
         <f>C27</f>
-        <v>0.31121951219512189</v>
+        <v>0.35365853658536578</v>
       </c>
       <c r="G27" s="24">
         <v>12500</v>
@@ -6771,10 +7810,10 @@
       </c>
       <c r="J27" s="42">
         <f>E27+G27+H27</f>
-        <v>791432.14948669705</v>
+        <v>732215.92085482879</v>
       </c>
       <c r="K27" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -6794,233 +7833,400 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="A29" s="24"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="12">
-        <v>10</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="24">
-        <f>J27</f>
-        <v>791432.14948669705</v>
-      </c>
-      <c r="F30" s="24">
-        <v>4</v>
-      </c>
-      <c r="G30" s="40">
-        <f>518*B30*(128/(2^(B30-1)))</f>
-        <v>1295</v>
-      </c>
-      <c r="H30" s="24">
-        <f>G30*J2</f>
-        <v>344.37290012514421</v>
-      </c>
-      <c r="I30">
-        <f>C27/F30</f>
-        <v>7.7804878048780474E-2</v>
-      </c>
-      <c r="J30" s="42">
-        <f>E30+H30+G30</f>
-        <v>793071.52238682215</v>
-      </c>
-      <c r="K30" t="s">
-        <v>121</v>
-      </c>
+      <c r="A30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="G31" s="39">
-        <v>1</v>
-      </c>
-      <c r="H31" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="I31" s="38">
-        <f>(I30)/G31</f>
-        <v>7.7804878048780474E-2</v>
-      </c>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="I32" s="38">
-        <f>I31*G31</f>
-        <v>7.7804878048780474E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="24"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
-      <c r="B33" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="24"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
       <c r="B34" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="12">
-        <f>780000+10000*B27</f>
-        <v>820000</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C34" s="24"/>
       <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
       <c r="B35" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" s="24">
-        <f>24*C27</f>
-        <v>7.4692682926829255</v>
+        <v>105</v>
+      </c>
+      <c r="C35" s="12">
+        <v>780000</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="42">
-        <f>(C34-J27)*C27</f>
-        <v>8890.8725012133073</v>
+        <v>124</v>
+      </c>
+      <c r="C36" s="24">
+        <f>24*C27</f>
+        <v>8.4878048780487791</v>
       </c>
       <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+      <c r="E36" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" t="s">
+        <v>135</v>
+      </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="42">
+        <f>(C35-J27)*C27</f>
+        <v>16899.247502560549</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I37" t="s">
+        <v>139</v>
+      </c>
+      <c r="K37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="42">
-        <f>C36*24</f>
-        <v>213380.94002911937</v>
-      </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
+      <c r="C38" s="42">
+        <f>C37*24</f>
+        <v>405581.94006145315</v>
+      </c>
       <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24" t="s">
+      <c r="E38" s="24">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>2426</v>
+      </c>
+      <c r="G38" s="44">
+        <f>$J$27/2800/F52</f>
+        <v>301.82024767305393</v>
+      </c>
+      <c r="H38" s="44">
+        <f>$J$27/2800/G52</f>
+        <v>298.86364116523629</v>
+      </c>
+      <c r="I38">
+        <f>(G38-H38)*$C$42</f>
+        <v>8278.4982218893892</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="E39" s="24">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>2604</v>
+      </c>
+      <c r="G39" s="44">
+        <f>$J$27/2800/F53</f>
+        <v>281.18890969847496</v>
+      </c>
+      <c r="H39" s="44">
+        <f>$J$27/2800/G53</f>
+        <v>278.93939842088719</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:I42" si="3">(G39-H39)*$C$42</f>
+        <v>6298.6315772457601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24" t="s">
+      <c r="C40" s="24"/>
+      <c r="E40" s="24">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>2699</v>
+      </c>
+      <c r="G40" s="44">
+        <f>$J$27/2800/F54</f>
+        <v>271.29156015369722</v>
+      </c>
+      <c r="H40" s="44">
+        <f>$J$27/2800/G54</f>
+        <v>269.94135331053599</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>3780.5791608514483</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C40" s="12">
-        <v>307</v>
-      </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24" t="s">
+      <c r="C41" s="12">
+        <v>282</v>
+      </c>
+      <c r="E41" s="24">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>2742</v>
+      </c>
+      <c r="G41" s="44">
+        <f>$J$27/2800/F55</f>
+        <v>267.03717026069614</v>
+      </c>
+      <c r="H41" s="44">
+        <f>$J$27/2800/G55</f>
+        <v>265.65656992465443</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>3865.6809409167863</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C42" s="24">
         <v>2800</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24" t="s">
+      <c r="E42" s="24">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>2765</v>
+      </c>
+      <c r="G42" s="44">
+        <f>$J$27/2800/F56</f>
+        <v>264.81588457679163</v>
+      </c>
+      <c r="H42" s="44">
+        <f>$J$27/2800/G56</f>
+        <v>263.56478590949968</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>3503.0762684174761</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="24">
-        <f>(0.5)^(B27+1)</f>
+      <c r="C43" s="24">
+        <f>LOOKUP(B27,E38:E42,F45:F49)</f>
+        <v>3.6071428571428532E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="1">
+        <f>C42*C41*(1-C43)</f>
+        <v>761118</v>
+      </c>
+      <c r="F44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="43">
+        <f>(C44-J27)*C27</f>
+        <v>10221.467014755672</v>
+      </c>
+      <c r="E45" s="24">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <f>1-F52</f>
+        <v>0.13357142857142856</v>
+      </c>
+      <c r="G45">
+        <f>1-G52</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="43">
+        <f>C45*24</f>
+        <v>245315.20835413612</v>
+      </c>
+      <c r="E46" s="24">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <f>1-F53</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="G46">
+        <f>1-G53</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E47" s="24">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <f>1-F54</f>
+        <v>3.6071428571428532E-2</v>
+      </c>
+      <c r="G47">
+        <f>1-G54</f>
         <v>3.125E-2</v>
       </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="1">
-        <f>C40*C41*(1-C42)</f>
-        <v>832737.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="43">
-        <f>(C43-J30)*C27</f>
-        <v>12344.826203515835</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C45" s="43">
-        <f>C44*24</f>
-        <v>296275.82888438005</v>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E48" s="24">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <f>1-F55</f>
+        <v>2.0714285714285685E-2</v>
+      </c>
+      <c r="G48">
+        <f>1-G55</f>
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="24">
+        <v>6</v>
+      </c>
+      <c r="F49">
+        <f>1-F56</f>
+        <v>1.2499999999999956E-2</v>
+      </c>
+      <c r="G49">
+        <f>1-G56</f>
+        <v>7.8125E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="24">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <f>F38/2800</f>
+        <v>0.86642857142857144</v>
+      </c>
+      <c r="G52">
+        <f>1- (0.5)^(E38+1)</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="24">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <f>F39/2800</f>
+        <v>0.93</v>
+      </c>
+      <c r="G53">
+        <f>1- (0.5)^(E39+1)</f>
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="24">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <f>F40/2800</f>
+        <v>0.96392857142857147</v>
+      </c>
+      <c r="G54">
+        <f>1- (0.5)^(E40+1)</f>
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="24">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <f>F41/2800</f>
+        <v>0.97928571428571431</v>
+      </c>
+      <c r="G55">
+        <f>1- (0.5)^(E41+1)</f>
+        <v>0.984375</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="24">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <f>F42/2800</f>
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="G56">
+        <f>1- (0.5)^(E42+1)</f>
+        <v>0.9921875</v>
       </c>
     </row>
   </sheetData>
@@ -7062,22 +8268,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="75.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7102,24 +8309,24 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="14">
-        <f>SUM(I20,I25,I29,I33)/170</f>
-        <v>0.24868449874738591</v>
+        <f>SUM(I20,I25,I32)/170</f>
+        <v>0.26590834698664634</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7135,19 +8342,19 @@
       </c>
       <c r="D3" s="4">
         <f>20*C18</f>
-        <v>232.00000000000003</v>
+        <v>255.184</v>
       </c>
       <c r="E3">
         <f>D3*24</f>
-        <v>5568.0000000000009</v>
+        <v>6124.4160000000002</v>
       </c>
       <c r="F3" s="41">
         <f t="shared" ref="F3:F10" si="0">D3*C3</f>
-        <v>2436.0000000000005</v>
+        <v>2679.4319999999998</v>
       </c>
       <c r="G3" s="41">
         <f>F3*24</f>
-        <v>58464.000000000015</v>
+        <v>64306.367999999995</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -7164,19 +8371,19 @@
       </c>
       <c r="D4" s="4">
         <f>8*C18</f>
-        <v>92.800000000000011</v>
+        <v>102.0736</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E10" si="1">D4*24</f>
-        <v>2227.2000000000003</v>
+        <v>2449.7664</v>
       </c>
       <c r="F4" s="41">
         <f t="shared" si="0"/>
-        <v>83520.000000000015</v>
+        <v>91866.240000000005</v>
       </c>
       <c r="G4" s="41">
         <f t="shared" ref="G4:G10" si="2">F4*24</f>
-        <v>2004480.0000000005</v>
+        <v>2204789.7600000002</v>
       </c>
       <c r="H4" s="4"/>
       <c r="L4" t="s">
@@ -7196,19 +8403,19 @@
       </c>
       <c r="D5" s="4">
         <f>10*C18</f>
-        <v>116.00000000000001</v>
+        <v>127.592</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2784.0000000000005</v>
+        <v>3062.2080000000001</v>
       </c>
       <c r="F5" s="41">
         <f t="shared" si="0"/>
-        <v>2146.0000000000005</v>
+        <v>2360.4519999999998</v>
       </c>
       <c r="G5" s="41">
         <f t="shared" si="2"/>
-        <v>51504.000000000015</v>
+        <v>56650.847999999998</v>
       </c>
       <c r="H5" s="4"/>
       <c r="L5" t="s">
@@ -7229,19 +8436,19 @@
       </c>
       <c r="D6" s="4">
         <f>40*C22</f>
-        <v>11.317073170731708</v>
+        <v>12.447999999999999</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>271.60975609756099</v>
+        <v>298.75199999999995</v>
       </c>
       <c r="F6" s="41">
         <f t="shared" si="0"/>
-        <v>35268.526829268296</v>
+        <v>38792.947199999995</v>
       </c>
       <c r="G6" s="41">
         <f t="shared" si="2"/>
-        <v>846444.64390243916</v>
+        <v>931030.73279999988</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -7259,19 +8466,19 @@
       </c>
       <c r="D7" s="4">
         <f>16*C22+C23*6</f>
-        <v>6.2243902439024392</v>
+        <v>6.8463999999999992</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>149.38536585365853</v>
+        <v>164.31359999999998</v>
       </c>
       <c r="F7" s="41">
         <f t="shared" si="0"/>
-        <v>60389.034146341466</v>
+        <v>66423.772799999992</v>
       </c>
       <c r="G7" s="41">
         <f t="shared" si="2"/>
-        <v>1449336.8195121952</v>
+        <v>1594170.5471999999</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -7288,19 +8495,19 @@
       </c>
       <c r="D8" s="4">
         <f>2*C23</f>
-        <v>0.56585365853658542</v>
+        <v>0.62239999999999995</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>13.58048780487805</v>
+        <v>14.9376</v>
       </c>
       <c r="F8" s="41">
         <f t="shared" si="0"/>
-        <v>3151.8048780487807</v>
+        <v>3466.7679999999996</v>
       </c>
       <c r="G8" s="41">
         <f t="shared" si="2"/>
-        <v>75643.317073170736</v>
+        <v>83202.431999999986</v>
       </c>
       <c r="H8" s="4"/>
       <c r="L8" s="38" t="s">
@@ -7323,19 +8530,19 @@
       </c>
       <c r="D9" s="4">
         <f>10*C23</f>
-        <v>2.8292682926829271</v>
+        <v>3.1119999999999997</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>67.902439024390247</v>
+        <v>74.687999999999988</v>
       </c>
       <c r="F9" s="41">
         <f t="shared" si="0"/>
-        <v>1541.9512195121954</v>
+        <v>1696.0399999999997</v>
       </c>
       <c r="G9" s="41">
         <f t="shared" si="2"/>
-        <v>37006.829268292691</v>
+        <v>40704.959999999992</v>
       </c>
       <c r="H9" s="4"/>
     </row>
@@ -7352,19 +8559,19 @@
       </c>
       <c r="D10" s="4">
         <f>4*C23</f>
-        <v>1.1317073170731708</v>
+        <v>1.2447999999999999</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>27.1609756097561</v>
+        <v>29.8752</v>
       </c>
       <c r="F10" s="41">
         <f t="shared" si="0"/>
-        <v>1957.8536585365855</v>
+        <v>2153.5039999999999</v>
       </c>
       <c r="G10" s="41">
         <f t="shared" si="2"/>
-        <v>46988.487804878052</v>
+        <v>51684.095999999998</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -7375,11 +8582,11 @@
       <c r="D11" s="4"/>
       <c r="F11" s="42">
         <f>SUM(F3:F10)</f>
-        <v>190411.17073170736</v>
+        <v>209439.15599999999</v>
       </c>
       <c r="G11" s="42">
-        <f>SUM(G3:G10)</f>
-        <v>4569868.0975609766</v>
+        <f>F11*24</f>
+        <v>5026539.7439999999</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -7424,7 +8631,7 @@
         <v>100</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>4</v>
@@ -7433,7 +8640,7 @@
         <v>84</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>7</v>
@@ -7477,7 +8684,7 @@
       </c>
       <c r="C18" s="24">
         <f>34*C22+7*C23</f>
-        <v>11.600000000000001</v>
+        <v>12.7592</v>
       </c>
       <c r="D18" s="27" t="s">
         <v>39</v>
@@ -7494,15 +8701,15 @@
       </c>
       <c r="H18" s="24">
         <f>$J$2*G18</f>
-        <v>494.73542865303699</v>
+        <v>529.00072457870408</v>
       </c>
       <c r="I18">
         <f>C18/F18</f>
-        <v>40.000000000000007</v>
+        <v>43.997241379310346</v>
       </c>
       <c r="J18" s="42">
         <f>E18+G18+H18</f>
-        <v>10079.145428653037</v>
+        <v>10113.410724578704</v>
       </c>
       <c r="K18" s="24"/>
       <c r="L18" s="4"/>
@@ -7518,14 +8725,14 @@
         <v>101</v>
       </c>
       <c r="G19" s="39">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" s="38" t="s">
         <v>102</v>
       </c>
       <c r="I19" s="38">
         <f>I18/G19</f>
-        <v>4.0000000000000009</v>
+        <v>3.9997492163009407</v>
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
@@ -7545,7 +8752,7 @@
       </c>
       <c r="I20" s="38">
         <f>I19*G19</f>
-        <v>40.000000000000007</v>
+        <v>43.997241379310346</v>
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
@@ -7578,14 +8785,14 @@
       </c>
       <c r="C22" s="4">
         <f>C27</f>
-        <v>0.28292682926829271</v>
+        <v>0.31119999999999998</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="4">
         <f>40*C6+16*C7+34*J18</f>
-        <v>622578.94457420334</v>
+        <v>623743.96463567601</v>
       </c>
       <c r="F22" s="4">
         <v>1.67</v>
@@ -7595,15 +8802,15 @@
       </c>
       <c r="H22" s="4">
         <f>$J$2*G22</f>
-        <v>87.449903984518244</v>
+        <v>93.506670217854179</v>
       </c>
       <c r="I22">
         <f>C22/F22</f>
-        <v>0.16941726303490581</v>
+        <v>0.18634730538922156</v>
       </c>
       <c r="J22" s="42">
         <f>E22+G22+H22</f>
-        <v>623018.04447818792</v>
+        <v>624189.12130589387</v>
       </c>
       <c r="K22" s="24"/>
       <c r="L22" s="4"/>
@@ -7619,14 +8826,14 @@
       </c>
       <c r="C23" s="4">
         <f>C27</f>
-        <v>0.28292682926829271</v>
+        <v>0.31119999999999998</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="4">
         <f>2*C8+10*C9+4*C10+6*C7+7*J18</f>
-        <v>152276.01800057126</v>
+        <v>152515.87507205093</v>
       </c>
       <c r="F23" s="4">
         <v>0.33</v>
@@ -7636,15 +8843,15 @@
       </c>
       <c r="H23" s="4">
         <f>$J$2*G23</f>
-        <v>437.2445462326163</v>
+        <v>467.52803292233119</v>
       </c>
       <c r="I23">
         <f>C23/F23</f>
-        <v>0.85735402808573546</v>
+        <v>0.94303030303030289</v>
       </c>
       <c r="J23" s="42">
         <f>E23+G23+H23</f>
-        <v>154471.4925468039</v>
+        <v>154741.63310497327</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="4"/>
@@ -7667,7 +8874,7 @@
       </c>
       <c r="I24" s="38">
         <f>(I22+I23)/G24</f>
-        <v>1.0267712911206412</v>
+        <v>1.1293776084195244</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
@@ -7687,7 +8894,7 @@
       </c>
       <c r="I25" s="38">
         <f>I24*G24</f>
-        <v>1.0267712911206412</v>
+        <v>1.1293776084195244</v>
       </c>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
@@ -7712,38 +8919,37 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="B27" s="12">
         <v>4</v>
       </c>
       <c r="C27" s="12">
-        <v>0.28292682926829271</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>48</v>
-      </c>
+        <v>0.31119999999999998</v>
+      </c>
+      <c r="D27" s="27"/>
       <c r="E27" s="24">
         <f>J22+J23</f>
-        <v>777489.53702499182</v>
+        <v>778930.75441086711</v>
       </c>
       <c r="F27" s="24">
-        <v>0.24</v>
+        <f>C27</f>
+        <v>0.31119999999999998</v>
       </c>
       <c r="G27" s="24">
-        <v>3170.85</v>
-      </c>
-      <c r="H27" s="24">
-        <f>$J$2*G27</f>
-        <v>788.54124285314856</v>
-      </c>
+        <v>12500</v>
+      </c>
+      <c r="H27" s="24"/>
       <c r="I27">
         <f>C27/F27</f>
-        <v>1.1788617886178863</v>
+        <v>1</v>
       </c>
       <c r="J27" s="42">
         <f>E27+G27+H27</f>
-        <v>781448.92826784495</v>
+        <v>791430.75441086711</v>
+      </c>
+      <c r="K27" t="s">
+        <v>131</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -7754,96 +8960,92 @@
       <c r="C28" s="24"/>
       <c r="D28" s="26"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="39">
-        <v>1</v>
-      </c>
-      <c r="H28" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="38">
-        <f>I27/G28</f>
-        <v>1.1788617886178863</v>
-      </c>
-      <c r="K28" t="s">
-        <v>126</v>
-      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" s="38">
-        <f>I28*G28</f>
-        <v>1.1788617886178863</v>
-      </c>
+      <c r="A29" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="J29" s="24"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="A30" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="12">
+        <v>8</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="24">
+        <f>J27</f>
+        <v>791430.75441086711</v>
+      </c>
+      <c r="F30" s="24">
+        <v>4</v>
+      </c>
+      <c r="G30" s="40">
+        <f>518*B30*(128/(2^(B30-1)))</f>
+        <v>4144</v>
+      </c>
+      <c r="H30" s="24">
+        <f>G30*J2</f>
+        <v>1101.9241899126623</v>
+      </c>
+      <c r="I30">
+        <f>C27/F30</f>
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="J30" s="42">
+        <f>E30+H30+G30</f>
+        <v>796676.67860077973</v>
+      </c>
+      <c r="K30" t="s">
+        <v>132</v>
+      </c>
+      <c r="L30" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="12">
-        <v>10</v>
-      </c>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="24"/>
-      <c r="D31" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="24">
-        <f>J27</f>
-        <v>781448.92826784495</v>
-      </c>
-      <c r="F31" s="24">
-        <v>4</v>
-      </c>
-      <c r="G31" s="40">
-        <f>518*B31*(128/(2^(B31-1)))</f>
-        <v>1295</v>
-      </c>
-      <c r="H31" s="24">
-        <f>G31*J2</f>
-        <v>322.04642587786475</v>
-      </c>
-      <c r="I31">
-        <f>C27/F31</f>
-        <v>7.0731707317073178E-2</v>
-      </c>
-      <c r="J31" s="42">
-        <f>E31+G31+H31</f>
-        <v>783065.97469372279</v>
-      </c>
-      <c r="K31" t="s">
-        <v>125</v>
+      <c r="D31" s="26"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="39">
+        <v>1</v>
+      </c>
+      <c r="H31" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" s="38">
+        <f>(I30)/G31</f>
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -7852,56 +9054,49 @@
       <c r="C32" s="24"/>
       <c r="D32" s="26"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="39">
-        <v>1</v>
-      </c>
+      <c r="G32" s="4"/>
       <c r="H32" s="38" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I32" s="38">
-        <f>(I31)/G32</f>
-        <v>7.0731707317073178E-2</v>
+        <f>I31*G31</f>
+        <v>7.7799999999999994E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
+      <c r="B33" s="24" t="s">
+        <v>109</v>
+      </c>
       <c r="C33" s="24"/>
       <c r="D33" s="26"/>
       <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="I33" s="38">
-        <f>I32*G32</f>
-        <v>7.0731707317073178E-2</v>
-      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="24"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
       <c r="B34" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="24"/>
+        <v>105</v>
+      </c>
+      <c r="C34" s="12">
+        <f>780000+10000*B27</f>
+        <v>820000</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
       <c r="B35" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="12">
-        <f>790000+15000*B27</f>
-        <v>850000</v>
+        <v>124</v>
+      </c>
+      <c r="C35" s="24">
+        <f>24*C27</f>
+        <v>7.4687999999999999</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -7910,11 +9105,11 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="24">
-        <f>24*C27</f>
-        <v>6.7902439024390251</v>
+        <v>106</v>
+      </c>
+      <c r="C36" s="42">
+        <f>(C34-J27)*C27</f>
+        <v>8890.749227338154</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -7923,31 +9118,27 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C37" s="42">
-        <f>(C35-J27)*C27</f>
-        <v>19394.937368121919</v>
+        <f>C36*24</f>
+        <v>213377.9814561157</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
-      <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
-      <c r="B38" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="42">
-        <f>C37*24</f>
-        <v>465478.49683492607</v>
-      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
+      <c r="B39" s="24" t="s">
+        <v>110</v>
+      </c>
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -7955,19 +9146,21 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="24"/>
+        <v>105</v>
+      </c>
+      <c r="C40" s="12">
+        <v>307</v>
+      </c>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="12">
-        <v>307</v>
+        <v>111</v>
+      </c>
+      <c r="C41" s="24">
+        <v>2800</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
@@ -7975,51 +9168,40 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C42" s="24">
-        <v>2800</v>
+        <f>(0.5)^(B27+1)</f>
+        <v>3.125E-2</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
       <c r="B43" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="24">
-        <f>(0.5)^(B27+1)</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+        <v>113</v>
+      </c>
+      <c r="C43" s="1">
+        <f>C40*C41*(1-C42)</f>
+        <v>832737.5</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="1">
-        <f>C41*C42*(1-C43)</f>
-        <v>832737.5</v>
+        <v>114</v>
+      </c>
+      <c r="C44" s="43">
+        <f>(C43-J30)*C27</f>
+        <v>11222.127619437346</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C45" s="43">
-        <f>(C44-J31)*C27</f>
-        <v>14053.407159824774</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="43">
-        <f>C45*24</f>
-        <v>337281.77183579456</v>
+        <f>C44*24</f>
+        <v>269331.06286649627</v>
       </c>
     </row>
   </sheetData>
@@ -8032,7 +9214,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7B01C992-87E0-4469-A5D5-96D18C7DB011}</x14:id>
+          <x14:id>{411ED40A-525F-48C3-BFFB-1C35E3AD0A01}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8043,7 +9225,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7B01C992-87E0-4469-A5D5-96D18C7DB011}">
+          <x14:cfRule type="dataBar" id="{411ED40A-525F-48C3-BFFB-1C35E3AD0A01}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
High production mining with low expected income.
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OF\Documents\GitHub\SimCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OF\Documents\SimCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -478,8 +478,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -713,7 +713,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -757,10 +757,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -6689,7 +6689,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7943,11 +7943,11 @@
         <v>2426</v>
       </c>
       <c r="G38" s="44">
-        <f>$J$27/2800/F52</f>
+        <f t="shared" ref="G38:H42" si="3">$J$27/2800/F52</f>
         <v>301.82024767305393</v>
       </c>
       <c r="H38" s="44">
-        <f>$J$27/2800/G52</f>
+        <f t="shared" si="3"/>
         <v>298.86364116523629</v>
       </c>
       <c r="I38">
@@ -7965,15 +7965,15 @@
         <v>2604</v>
       </c>
       <c r="G39" s="44">
-        <f>$J$27/2800/F53</f>
+        <f t="shared" si="3"/>
         <v>281.18890969847496</v>
       </c>
       <c r="H39" s="44">
-        <f>$J$27/2800/G53</f>
+        <f t="shared" si="3"/>
         <v>278.93939842088719</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I42" si="3">(G39-H39)*$C$42</f>
+        <f t="shared" ref="I39:I42" si="4">(G39-H39)*$C$42</f>
         <v>6298.6315772457601</v>
       </c>
     </row>
@@ -7989,15 +7989,15 @@
         <v>2699</v>
       </c>
       <c r="G40" s="44">
-        <f>$J$27/2800/F54</f>
+        <f t="shared" si="3"/>
         <v>271.29156015369722</v>
       </c>
       <c r="H40" s="44">
-        <f>$J$27/2800/G54</f>
+        <f t="shared" si="3"/>
         <v>269.94135331053599</v>
       </c>
       <c r="I40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3780.5791608514483</v>
       </c>
     </row>
@@ -8015,15 +8015,15 @@
         <v>2742</v>
       </c>
       <c r="G41" s="44">
-        <f>$J$27/2800/F55</f>
+        <f t="shared" si="3"/>
         <v>267.03717026069614</v>
       </c>
       <c r="H41" s="44">
-        <f>$J$27/2800/G55</f>
+        <f t="shared" si="3"/>
         <v>265.65656992465443</v>
       </c>
       <c r="I41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3865.6809409167863</v>
       </c>
     </row>
@@ -8041,15 +8041,15 @@
         <v>2765</v>
       </c>
       <c r="G42" s="44">
-        <f>$J$27/2800/F56</f>
+        <f t="shared" si="3"/>
         <v>264.81588457679163</v>
       </c>
       <c r="H42" s="44">
-        <f>$J$27/2800/G56</f>
+        <f t="shared" si="3"/>
         <v>263.56478590949968</v>
       </c>
       <c r="I42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3503.0762684174761</v>
       </c>
     </row>
@@ -8089,11 +8089,11 @@
         <v>2</v>
       </c>
       <c r="F45">
-        <f>1-F52</f>
+        <f t="shared" ref="F45:G49" si="5">1-F52</f>
         <v>0.13357142857142856</v>
       </c>
       <c r="G45">
-        <f>1-G52</f>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
     </row>
@@ -8109,11 +8109,11 @@
         <v>3</v>
       </c>
       <c r="F46">
-        <f>1-F53</f>
+        <f t="shared" si="5"/>
         <v>6.9999999999999951E-2</v>
       </c>
       <c r="G46">
-        <f>1-G53</f>
+        <f t="shared" si="5"/>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -8122,11 +8122,11 @@
         <v>4</v>
       </c>
       <c r="F47">
-        <f>1-F54</f>
+        <f t="shared" si="5"/>
         <v>3.6071428571428532E-2</v>
       </c>
       <c r="G47">
-        <f>1-G54</f>
+        <f t="shared" si="5"/>
         <v>3.125E-2</v>
       </c>
     </row>
@@ -8135,11 +8135,11 @@
         <v>5</v>
       </c>
       <c r="F48">
-        <f>1-F55</f>
+        <f t="shared" si="5"/>
         <v>2.0714285714285685E-2</v>
       </c>
       <c r="G48">
-        <f>1-G55</f>
+        <f t="shared" si="5"/>
         <v>1.5625E-2</v>
       </c>
     </row>
@@ -8148,11 +8148,11 @@
         <v>6</v>
       </c>
       <c r="F49">
-        <f>1-F56</f>
+        <f t="shared" si="5"/>
         <v>1.2499999999999956E-2</v>
       </c>
       <c r="G49">
-        <f>1-G56</f>
+        <f t="shared" si="5"/>
         <v>7.8125E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
admin overhead problems :(
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All of them" sheetId="12" r:id="rId1"/>
@@ -23,6 +23,38 @@
     <sheet name="Production Plans third stage" sheetId="16" r:id="rId9"/>
     <sheet name="Production Plans final stage" sheetId="14" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'Rocket production'!$C$13</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'Rocket production'!$B$31</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'Rocket production'!$C$20</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">0.02</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="152">
   <si>
     <t>Carbon composite</t>
   </si>
@@ -471,6 +503,24 @@
   </si>
   <si>
     <t>We will also pay someoune to launch our BFRs</t>
+  </si>
+  <si>
+    <t>Propulsion factory building price</t>
+  </si>
+  <si>
+    <t>Total buildings price</t>
+  </si>
+  <si>
+    <t>COO skill</t>
+  </si>
+  <si>
+    <t>Adjusted adm. Overhead</t>
+  </si>
+  <si>
+    <t>COO discount overhead</t>
+  </si>
+  <si>
+    <t>earnings / buildings value</t>
   </si>
 </sst>
 </file>
@@ -715,7 +765,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -761,6 +811,8 @@
     <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -4734,8 +4786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6686,10 +6738,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6702,7 +6754,7 @@
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -6739,12 +6791,12 @@
         <v>121</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="14">
-        <f>I15/170</f>
-        <v>0.32941176470588235</v>
+      <c r="J2" s="4">
+        <f>I13/170</f>
+        <v>0.38240000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6756,25 +6808,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="12">
-        <v>10.9</v>
+        <v>10.5</v>
       </c>
       <c r="D3" s="4">
         <f>20*C13</f>
-        <v>324.79999999999995</v>
+        <v>377.04640000000006</v>
       </c>
       <c r="E3">
         <f>D3*24</f>
-        <v>7795.1999999999989</v>
+        <v>9049.1136000000006</v>
       </c>
       <c r="F3" s="41">
         <f>D3*C3</f>
-        <v>3540.3199999999997</v>
+        <v>3958.9872000000005</v>
       </c>
       <c r="G3" s="41">
         <f>F3*24</f>
-        <v>84967.679999999993</v>
+        <v>95015.692800000019</v>
       </c>
       <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J3" s="12">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -6785,25 +6843,32 @@
         <v>2</v>
       </c>
       <c r="C4" s="12">
-        <v>820</v>
+        <v>890</v>
       </c>
       <c r="D4" s="4">
         <f>8*C13</f>
-        <v>129.91999999999999</v>
+        <v>150.81856000000002</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E5" si="0">D4*24</f>
-        <v>3118.08</v>
+        <v>3619.6454400000002</v>
       </c>
       <c r="F4" s="41">
         <f>D4*C4</f>
-        <v>106534.39999999999</v>
+        <v>134228.51840000003</v>
       </c>
       <c r="G4" s="41">
         <f t="shared" ref="G4:G5" si="1">F4*24</f>
-        <v>2556825.5999999996</v>
+        <v>3221484.4416000005</v>
       </c>
       <c r="H4" s="4"/>
+      <c r="I4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J4">
+        <f>J3*J2/100</f>
+        <v>5.3536000000000007E-2</v>
+      </c>
       <c r="L4" t="s">
         <v>97</v>
       </c>
@@ -6817,25 +6882,32 @@
         <v>2</v>
       </c>
       <c r="C5" s="12">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4">
         <f>10*C13</f>
-        <v>162.39999999999998</v>
+        <v>188.52320000000003</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>3897.5999999999995</v>
+        <v>4524.5568000000003</v>
       </c>
       <c r="F5" s="41">
         <f>D5*C5</f>
-        <v>3085.5999999999995</v>
+        <v>3393.4176000000007</v>
       </c>
       <c r="G5" s="41">
         <f t="shared" si="1"/>
-        <v>74054.399999999994</v>
+        <v>81442.022400000016</v>
       </c>
       <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" s="4">
+        <f>J2-J4</f>
+        <v>0.32886400000000005</v>
+      </c>
       <c r="L5" t="s">
         <v>98</v>
       </c>
@@ -6849,11 +6921,11 @@
       <c r="D6" s="4"/>
       <c r="F6" s="41">
         <f>(G13+H13)*C13</f>
-        <v>42950.659755294117</v>
+        <v>49839.036255390165</v>
       </c>
       <c r="G6" s="41">
         <f>F6*24</f>
-        <v>1030815.8341270587</v>
+        <v>1196136.8701293641</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -6864,11 +6936,11 @@
       <c r="D7" s="4"/>
       <c r="F7" s="42">
         <f>SUM(F3:F6)</f>
-        <v>156110.97975529413</v>
+        <v>191419.95945539017</v>
       </c>
       <c r="G7" s="42">
         <f>SUM(G3:G6)</f>
-        <v>3746663.5141270584</v>
+        <v>4594079.0269293645</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -6956,14 +7028,14 @@
         <v>3</v>
       </c>
       <c r="C13" s="12">
-        <v>16.239999999999998</v>
+        <v>18.852320000000002</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="24">
         <f>20*C3+8*C4+10*C5</f>
-        <v>6968</v>
+        <v>7510</v>
       </c>
       <c r="F13" s="24">
         <v>0.28999999999999998</v>
@@ -6972,16 +7044,16 @@
         <v>1989.41</v>
       </c>
       <c r="H13" s="24">
-        <f>$J$2*G13</f>
-        <v>655.33505882352938</v>
+        <f>$J$5*G13</f>
+        <v>654.24533024000016</v>
       </c>
       <c r="I13">
         <f>C13/F13</f>
-        <v>56</v>
+        <v>65.00800000000001</v>
       </c>
       <c r="J13" s="42">
         <f>E13+G13+H13</f>
-        <v>9612.7450588235297</v>
+        <v>10153.655330240001</v>
       </c>
       <c r="K13" s="24"/>
       <c r="L13" s="4"/>
@@ -7004,7 +7076,7 @@
       </c>
       <c r="I14" s="38">
         <f>I13/G14</f>
-        <v>4.3076923076923075</v>
+        <v>5.0006153846153856</v>
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="24" t="s">
@@ -7024,7 +7096,7 @@
       </c>
       <c r="I15" s="38">
         <f>I14*G14</f>
-        <v>56</v>
+        <v>65.00800000000001</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -7040,7 +7112,7 @@
         <v>105</v>
       </c>
       <c r="C17" s="12">
-        <v>10600</v>
+        <v>11300</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
@@ -7052,7 +7124,7 @@
       </c>
       <c r="C18" s="24">
         <f>C13*24</f>
-        <v>389.76</v>
+        <v>452.45568000000003</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -7064,7 +7136,7 @@
       </c>
       <c r="C19" s="42">
         <f>(C17-J13)*C13</f>
-        <v>16033.020244705876</v>
+        <v>21611.256544609834</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -7076,7 +7148,7 @@
       </c>
       <c r="C20" s="42">
         <f>C19*24</f>
-        <v>384792.48587294103</v>
+        <v>518670.15707063605</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -7094,6 +7166,32 @@
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="45">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="46">
+        <f>((I14+1)*I14/2+1)*B29*G14</f>
+        <v>21844620.258461546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="21">
+        <f>C20/B30</f>
+        <v>2.3743610597658633E-2</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M11:M12">
@@ -7136,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Analytical solution to the Optimal building level. ipynb
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -6823,7 +6823,7 @@
       </c>
       <c r="J2" s="4">
         <f>I15/170</f>
-        <v>0.40567951318458423</v>
+        <v>0.36975997295469903</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6839,19 +6839,19 @@
       </c>
       <c r="D3" s="4">
         <f>20*C13</f>
-        <v>400</v>
+        <v>364.58333333333326</v>
       </c>
       <c r="E3">
         <f>D3*24</f>
-        <v>9600</v>
+        <v>8749.9999999999982</v>
       </c>
       <c r="F3" s="38">
         <f>D3*C3</f>
-        <v>4360</v>
+        <v>3973.9583333333326</v>
       </c>
       <c r="G3" s="38">
         <f>F3*24</f>
-        <v>104640</v>
+        <v>95374.999999999985</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
@@ -6878,19 +6878,19 @@
       </c>
       <c r="D4" s="4">
         <f>8*C13</f>
-        <v>160</v>
+        <v>145.83333333333331</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E5" si="0">D4*24</f>
-        <v>3840</v>
+        <v>3499.9999999999995</v>
       </c>
       <c r="F4" s="38">
         <f>D4*C4</f>
-        <v>142400</v>
+        <v>129791.66666666666</v>
       </c>
       <c r="G4" s="38">
         <f t="shared" ref="G4:G5" si="1">F4*24</f>
-        <v>3417600</v>
+        <v>3115000</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" t="s">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="J4">
         <f>J3*J2/100</f>
-        <v>0.1054766734279919</v>
+        <v>9.6137592968221761E-2</v>
       </c>
       <c r="L4" t="s">
         <v>96</v>
@@ -6917,19 +6917,19 @@
       </c>
       <c r="D5" s="4">
         <f>10*C13</f>
-        <v>200</v>
+        <v>182.29166666666663</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>4800</v>
+        <v>4374.9999999999991</v>
       </c>
       <c r="F5" s="38">
         <f>D5*C5</f>
-        <v>3600</v>
+        <v>3281.2499999999991</v>
       </c>
       <c r="G5" s="38">
         <f t="shared" si="1"/>
-        <v>86400</v>
+        <v>78749.999999999971</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
@@ -6937,7 +6937,7 @@
       </c>
       <c r="J5" s="4">
         <f>J2-J4</f>
-        <v>0.30020283975659234</v>
+        <v>0.27362237998647726</v>
       </c>
       <c r="L5" t="s">
         <v>97</v>
@@ -6952,11 +6952,11 @@
       <c r="D6" s="4"/>
       <c r="F6" s="38">
         <f>(G13+H13)*C13</f>
-        <v>57755.010141987834</v>
+        <v>51565.122764712913</v>
       </c>
       <c r="G6" s="38">
         <f>F6*24</f>
-        <v>1386120.2434077081</v>
+        <v>1237562.94635311</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -6969,11 +6969,11 @@
       <c r="D7" s="4"/>
       <c r="F7" s="39">
         <f>SUM(F3:F6)</f>
-        <v>208115.01014198782</v>
+        <v>188611.9977647129</v>
       </c>
       <c r="G7" s="39">
         <f>SUM(G3:G6)</f>
-        <v>4994760.2434077077</v>
+        <v>4526687.9463531096</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -7063,7 +7063,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="12">
-        <v>20</v>
+        <v>18.229166666666664</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>39</v>
@@ -7080,15 +7080,15 @@
       </c>
       <c r="H13" s="22">
         <f>$J$5*G13</f>
-        <v>666.7505070993916</v>
+        <v>607.71530594996602</v>
       </c>
       <c r="I13">
         <f>C13/F13</f>
-        <v>68.965517241379317</v>
+        <v>62.859195402298845</v>
       </c>
       <c r="J13" s="39">
         <f>E13+G13+H13</f>
-        <v>10405.750507099392</v>
+        <v>10346.715305949965</v>
       </c>
       <c r="K13" s="22"/>
       <c r="L13" s="4"/>
@@ -7104,14 +7104,14 @@
         <v>100</v>
       </c>
       <c r="G14" s="37">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="36" t="s">
         <v>101</v>
       </c>
       <c r="I14" s="36">
         <f>I13/G14</f>
-        <v>4.9261083743842367</v>
+        <v>4.835322723253757</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22" t="s">
@@ -7131,7 +7131,7 @@
       </c>
       <c r="I15" s="36">
         <f>I14*G14</f>
-        <v>68.965517241379317</v>
+        <v>62.859195402298838</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -7159,7 +7159,7 @@
       </c>
       <c r="C18" s="19">
         <f>C21/C19/C17</f>
-        <v>9.5152129817444184E-2</v>
+        <v>0.10028562556956826</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -7171,7 +7171,7 @@
       </c>
       <c r="C19" s="22">
         <f>C13*24</f>
-        <v>480</v>
+        <v>437.49999999999994</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -7183,7 +7183,7 @@
       </c>
       <c r="C20" s="39">
         <f>(C17-J13)*C13</f>
-        <v>21884.989858012159</v>
+        <v>21023.418901953759</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="C21" s="39">
         <f>C20*24</f>
-        <v>525239.75659229187</v>
+        <v>504562.05364689021</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -7241,7 +7241,7 @@
       </c>
       <c r="B30" s="43">
         <f>((I14+1)*I14/2+1)*B29*G14</f>
-        <v>22926599.286563616</v>
+        <v>20622193.793065332</v>
       </c>
       <c r="C30" t="s">
         <v>151</v>
@@ -7253,7 +7253,7 @@
       </c>
       <c r="B31" s="19">
         <f>C21/B30</f>
-        <v>2.2909623447735415E-2</v>
+        <v>2.4466943658368701E-2</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Various Multi-step processes simulated
Thinking about multiple products, with multiple steps...
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All of them" sheetId="12" r:id="rId1"/>
@@ -4813,8 +4813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6768,7 +6768,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="J2" s="4">
         <f>I15/170</f>
-        <v>0.30588235294117649</v>
+        <v>0.29213705684293922</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6839,26 +6839,26 @@
       </c>
       <c r="D3" s="4">
         <f>20*C13</f>
-        <v>301.59999999999997</v>
+        <v>295</v>
       </c>
       <c r="E3">
         <f>D3*24</f>
-        <v>7238.4</v>
+        <v>7080</v>
       </c>
       <c r="F3" s="38">
         <f>D3*C3</f>
-        <v>3287.4399999999996</v>
+        <v>3215.5</v>
       </c>
       <c r="G3" s="38">
         <f>F3*24</f>
-        <v>78898.559999999998</v>
+        <v>77172</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
         <v>145</v>
       </c>
       <c r="J3" s="12">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="K3">
         <f>18+(16+7+12)/4</f>
@@ -6878,19 +6878,19 @@
       </c>
       <c r="D4" s="4">
         <f>8*C13</f>
-        <v>120.63999999999999</v>
+        <v>118</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E5" si="0">D4*24</f>
-        <v>2895.3599999999997</v>
+        <v>2832</v>
       </c>
       <c r="F4" s="38">
         <f>D4*C4</f>
-        <v>107369.59999999999</v>
+        <v>105020</v>
       </c>
       <c r="G4" s="38">
         <f t="shared" ref="G4:G5" si="1">F4*24</f>
-        <v>2576870.3999999999</v>
+        <v>2520480</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" t="s">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="J4">
         <f>J3*J2/100</f>
-        <v>7.952941176470589E-2</v>
+        <v>0.10224796989502873</v>
       </c>
       <c r="L4" t="s">
         <v>96</v>
@@ -6917,19 +6917,19 @@
       </c>
       <c r="D5" s="4">
         <f>10*C13</f>
-        <v>150.79999999999998</v>
+        <v>147.5</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>3619.2</v>
+        <v>3540</v>
       </c>
       <c r="F5" s="38">
         <f>D5*C5</f>
-        <v>2714.3999999999996</v>
+        <v>2655</v>
       </c>
       <c r="G5" s="38">
         <f t="shared" si="1"/>
-        <v>65145.599999999991</v>
+        <v>63720</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
@@ -6937,7 +6937,7 @@
       </c>
       <c r="J5" s="4">
         <f>J2-J4</f>
-        <v>0.22635294117647059</v>
+        <v>0.18988908694791051</v>
       </c>
       <c r="L5" t="s">
         <v>97</v>
@@ -6952,11 +6952,11 @@
       <c r="D6" s="4"/>
       <c r="F6" s="38">
         <f>(G13+H13)*C13</f>
-        <v>41073.846625882354</v>
+        <v>38945.36728807685</v>
       </c>
       <c r="G6" s="38">
         <f>F6*24</f>
-        <v>985772.31902117655</v>
+        <v>934688.81491384446</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -6969,11 +6969,11 @@
       <c r="D7" s="4"/>
       <c r="F7" s="39">
         <f>SUM(F3:F6)</f>
-        <v>154445.28662588235</v>
+        <v>149835.86728807684</v>
       </c>
       <c r="G7" s="39">
         <f>SUM(G3:G6)</f>
-        <v>3706686.8790211766</v>
+        <v>3596060.8149138447</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -7063,8 +7063,8 @@
         <v>3</v>
       </c>
       <c r="C13" s="12">
-        <f>0.29*52</f>
-        <v>15.079999999999998</v>
+        <f>0.295*50</f>
+        <v>14.75</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>39</v>
@@ -7074,22 +7074,22 @@
         <v>7518</v>
       </c>
       <c r="F13" s="22">
-        <v>0.28999999999999998</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="G13" s="44">
-        <v>2221</v>
+        <v>2219</v>
       </c>
       <c r="H13" s="22">
         <f>$J$5*G13</f>
-        <v>502.72988235294116</v>
+        <v>421.36388393741345</v>
       </c>
       <c r="I13">
         <f>C13/F13</f>
-        <v>52</v>
+        <v>49.663299663299668</v>
       </c>
       <c r="J13" s="39">
         <f>E13+G13+H13</f>
-        <v>10241.729882352942</v>
+        <v>10158.363883937414</v>
       </c>
       <c r="K13" s="22"/>
       <c r="L13" s="4"/>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="I14" s="36">
         <f>I13/G14</f>
-        <v>4</v>
+        <v>3.8202538202538205</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22" t="s">
@@ -7132,7 +7132,7 @@
       </c>
       <c r="I15" s="36">
         <f>I14*G14</f>
-        <v>52</v>
+        <v>49.663299663299668</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -7160,7 +7160,7 @@
       </c>
       <c r="C18" s="19">
         <f>C21/C19/C17</f>
-        <v>0.10941479283887463</v>
+        <v>0.11666401009239875</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="C19" s="22">
         <f>C13*24</f>
-        <v>361.91999999999996</v>
+        <v>354</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -7184,7 +7184,7 @@
       </c>
       <c r="C20" s="39">
         <f>(C17-J13)*C13</f>
-        <v>18974.713374117637</v>
+        <v>19789.132711923139</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -7196,7 +7196,7 @@
       </c>
       <c r="C21" s="39">
         <f>C20*24</f>
-        <v>455393.12097882328</v>
+        <v>474939.18508615531</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -7242,7 +7242,7 @@
       </c>
       <c r="B30" s="43">
         <f>(1+((I14/2)*(I14-1)))*B29*G14</f>
-        <v>9555000</v>
+        <v>8718313.3065961357</v>
       </c>
       <c r="C30" t="s">
         <v>151</v>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="B31" s="19">
         <f>C21/B30</f>
-        <v>4.7660190578631426E-2</v>
+        <v>5.4476040076103245E-2</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Production speed bonus adjustments
</commit_message>
<xml_diff>
--- a/sim companies.xlsx
+++ b/sim companies.xlsx
@@ -6768,7 +6768,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="J2" s="4">
         <f>I15/170</f>
-        <v>0.29213705684293922</v>
+        <v>0.29511804721888751</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="J4">
         <f>J3*J2/100</f>
-        <v>0.10224796989502873</v>
+        <v>0.10329131652661064</v>
       </c>
       <c r="L4" t="s">
         <v>96</v>
@@ -6937,7 +6937,7 @@
       </c>
       <c r="J5" s="4">
         <f>J2-J4</f>
-        <v>0.18988908694791051</v>
+        <v>0.19182673069227688</v>
       </c>
       <c r="L5" t="s">
         <v>97</v>
@@ -6952,11 +6952,11 @@
       <c r="D6" s="4"/>
       <c r="F6" s="38">
         <f>(G13+H13)*C13</f>
-        <v>38945.36728807685</v>
+        <v>39008.786852240897</v>
       </c>
       <c r="G6" s="38">
         <f>F6*24</f>
-        <v>934688.81491384446</v>
+        <v>936210.88445378153</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -6969,11 +6969,11 @@
       <c r="D7" s="4"/>
       <c r="F7" s="39">
         <f>SUM(F3:F6)</f>
-        <v>149835.86728807684</v>
+        <v>149899.28685224091</v>
       </c>
       <c r="G7" s="39">
         <f>SUM(G3:G6)</f>
-        <v>3596060.8149138447</v>
+        <v>3597582.8844537814</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -7074,22 +7074,23 @@
         <v>7518</v>
       </c>
       <c r="F13" s="22">
-        <v>0.29699999999999999</v>
+        <f>0.28*1.05</f>
+        <v>0.29400000000000004</v>
       </c>
       <c r="G13" s="44">
         <v>2219</v>
       </c>
       <c r="H13" s="22">
         <f>$J$5*G13</f>
-        <v>421.36388393741345</v>
+        <v>425.66351540616239</v>
       </c>
       <c r="I13">
         <f>C13/F13</f>
-        <v>49.663299663299668</v>
+        <v>50.170068027210881</v>
       </c>
       <c r="J13" s="39">
         <f>E13+G13+H13</f>
-        <v>10158.363883937414</v>
+        <v>10162.663515406162</v>
       </c>
       <c r="K13" s="22"/>
       <c r="L13" s="4"/>
@@ -7112,7 +7113,7 @@
       </c>
       <c r="I14" s="36">
         <f>I13/G14</f>
-        <v>3.8202538202538205</v>
+        <v>3.8592360020931449</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22" t="s">
@@ -7132,7 +7133,7 @@
       </c>
       <c r="I15" s="36">
         <f>I14*G14</f>
-        <v>49.663299663299668</v>
+        <v>50.170068027210881</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -7160,7 +7161,7 @@
       </c>
       <c r="C18" s="19">
         <f>C21/C19/C17</f>
-        <v>0.11666401009239875</v>
+        <v>0.11629012909511634</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -7184,7 +7185,7 @@
       </c>
       <c r="C20" s="39">
         <f>(C17-J13)*C13</f>
-        <v>19789.132711923139</v>
+        <v>19725.713147759107</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -7196,7 +7197,7 @@
       </c>
       <c r="C21" s="39">
         <f>C20*24</f>
-        <v>474939.18508615531</v>
+        <v>473417.11554621859</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -7242,7 +7243,7 @@
       </c>
       <c r="B30" s="43">
         <f>(1+((I14/2)*(I14-1)))*B29*G14</f>
-        <v>8718313.3065961357</v>
+        <v>8896023.3983703367</v>
       </c>
       <c r="C30" t="s">
         <v>151</v>
@@ -7254,7 +7255,7 @@
       </c>
       <c r="B31" s="19">
         <f>C21/B30</f>
-        <v>5.4476040076103245E-2</v>
+        <v>5.3216712046074865E-2</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>